<commit_message>
improved calculater UI and function
</commit_message>
<xml_diff>
--- a/data/Metadata.xlsx
+++ b/data/Metadata.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yifu/Documents/github-repo/iibr-pmrt-calculator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A717F507-45EC-FC40-9232-12E074F0F0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2040FCB-4D0B-F54D-AEDF-A0651B803FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{2D76DBCA-B48D-704D-8521-B15612E5208C}"/>
+    <workbookView xWindow="3920" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{2D76DBCA-B48D-704D-8521-B15612E5208C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$124</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$125</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -66,7 +66,7 @@
     <author>tc={1E3217F0-059D-9B4A-891F-86093E663007}</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{E88C6DA9-1AC2-0947-AA4C-0A0AE69DB287}">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{E88C6DA9-1AC2-0947-AA4C-0A0AE69DB287}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -74,7 +74,7 @@
     replace unknown (3) with missing, so that we can impute</t>
       </text>
     </comment>
-    <comment ref="E3" authorId="1" shapeId="0" xr:uid="{0851E83E-F569-CC48-8979-68324726D851}">
+    <comment ref="E4" authorId="1" shapeId="0" xr:uid="{0851E83E-F569-CC48-8979-68324726D851}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -82,7 +82,7 @@
     Impute not palpable (0)</t>
       </text>
     </comment>
-    <comment ref="A5" authorId="2" shapeId="0" xr:uid="{90142F8C-850A-2045-B460-594C957F7CEE}">
+    <comment ref="A6" authorId="2" shapeId="0" xr:uid="{90142F8C-850A-2045-B460-594C957F7CEE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -90,7 +90,7 @@
     unexpected missingness; to be chart-reviewed</t>
       </text>
     </comment>
-    <comment ref="J5" authorId="3" shapeId="0" xr:uid="{F44E1E05-68FC-C345-A086-9513C71E467A}">
+    <comment ref="J6" authorId="3" shapeId="0" xr:uid="{F44E1E05-68FC-C345-A086-9513C71E467A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -98,7 +98,7 @@
     unexpected missingness; to be chart-reviewed</t>
       </text>
     </comment>
-    <comment ref="E8" authorId="4" shapeId="0" xr:uid="{4E0ABAC6-E2DE-4D45-B44A-4E24BE55D192}">
+    <comment ref="E9" authorId="4" shapeId="0" xr:uid="{4E0ABAC6-E2DE-4D45-B44A-4E24BE55D192}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -106,7 +106,7 @@
     impute 0 if blank</t>
       </text>
     </comment>
-    <comment ref="E9" authorId="5" shapeId="0" xr:uid="{5701CC43-81B2-5C4D-9C08-77ACBE9D2AB9}">
+    <comment ref="E10" authorId="5" shapeId="0" xr:uid="{5701CC43-81B2-5C4D-9C08-77ACBE9D2AB9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -116,7 +116,7 @@
     TODO: Choose larger among img_size and tumor_size_mm</t>
       </text>
     </comment>
-    <comment ref="D10" authorId="6" shapeId="0" xr:uid="{BE8AC716-1D1C-B642-BED8-C425D517B077}">
+    <comment ref="D11" authorId="6" shapeId="0" xr:uid="{BE8AC716-1D1C-B642-BED8-C425D517B077}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -124,7 +124,7 @@
     replace not mentioned with no</t>
       </text>
     </comment>
-    <comment ref="E10" authorId="7" shapeId="0" xr:uid="{EEB800EB-04A9-0E4C-89C5-508F14B60227}">
+    <comment ref="E11" authorId="7" shapeId="0" xr:uid="{EEB800EB-04A9-0E4C-89C5-508F14B60227}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -132,7 +132,7 @@
     if blank, impute 2 (No). Replace 3 by 2.</t>
       </text>
     </comment>
-    <comment ref="E11" authorId="8" shapeId="0" xr:uid="{98281554-B8B9-5C4C-8250-32226D76D614}">
+    <comment ref="E12" authorId="8" shapeId="0" xr:uid="{98281554-B8B9-5C4C-8250-32226D76D614}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -140,7 +140,7 @@
     TODO: Construct a new column with img_size, take the more authoritative measurement</t>
       </text>
     </comment>
-    <comment ref="E13" authorId="9" shapeId="0" xr:uid="{4031F437-0C18-9A40-A568-C9BC83920B49}">
+    <comment ref="E14" authorId="9" shapeId="0" xr:uid="{4031F437-0C18-9A40-A568-C9BC83920B49}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -148,7 +148,7 @@
     TODO: Construct a new column with lymph_node_max_size_mm </t>
       </text>
     </comment>
-    <comment ref="E14" authorId="10" shapeId="0" xr:uid="{D7EDEE7B-587E-D848-8C5D-279BA8E53A36}">
+    <comment ref="E15" authorId="10" shapeId="0" xr:uid="{D7EDEE7B-587E-D848-8C5D-279BA8E53A36}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -156,7 +156,7 @@
     drop variable because ultrasound is better?</t>
       </text>
     </comment>
-    <comment ref="E15" authorId="11" shapeId="0" xr:uid="{E1553B31-F607-BE4A-81A5-7BBE8308D7DF}">
+    <comment ref="E16" authorId="11" shapeId="0" xr:uid="{E1553B31-F607-BE4A-81A5-7BBE8308D7DF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -164,7 +164,7 @@
     impute 0 if blank, convert to binary variable</t>
       </text>
     </comment>
-    <comment ref="E39" authorId="12" shapeId="0" xr:uid="{04ADA115-B14D-1848-B5AE-2A1C3D5ED21A}">
+    <comment ref="E40" authorId="12" shapeId="0" xr:uid="{04ADA115-B14D-1848-B5AE-2A1C3D5ED21A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -172,7 +172,7 @@
     TODO: group 2 and 3 together; 4 and 5 together</t>
       </text>
     </comment>
-    <comment ref="E54" authorId="13" shapeId="0" xr:uid="{707F85C7-4A70-8445-AD41-E181BA97C713}">
+    <comment ref="E55" authorId="13" shapeId="0" xr:uid="{707F85C7-4A70-8445-AD41-E181BA97C713}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -181,7 +181,7 @@
 Impute: Jan 2020"</t>
       </text>
     </comment>
-    <comment ref="E62" authorId="14" shapeId="0" xr:uid="{35A6CD70-95AF-CA4E-AD09-29213DDCD3C0}">
+    <comment ref="E63" authorId="14" shapeId="0" xr:uid="{35A6CD70-95AF-CA4E-AD09-29213DDCD3C0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -189,7 +189,7 @@
     impute 0 if blank</t>
       </text>
     </comment>
-    <comment ref="E64" authorId="15" shapeId="0" xr:uid="{E7E014ED-CA32-CF4B-B7EA-09A950207112}">
+    <comment ref="E65" authorId="15" shapeId="0" xr:uid="{E7E014ED-CA32-CF4B-B7EA-09A950207112}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -197,7 +197,7 @@
     ie don’t manually impute</t>
       </text>
     </comment>
-    <comment ref="E65" authorId="16" shapeId="0" xr:uid="{CFBAAC2D-21C1-684D-9816-483DFFD98BA2}">
+    <comment ref="E66" authorId="16" shapeId="0" xr:uid="{CFBAAC2D-21C1-684D-9816-483DFFD98BA2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -205,7 +205,7 @@
     impute 1 (most are unifocal), replace 0 with 1.</t>
       </text>
     </comment>
-    <comment ref="E66" authorId="17" shapeId="0" xr:uid="{28EAF8C7-F361-7B4A-983B-19A1D1C30C81}">
+    <comment ref="E67" authorId="17" shapeId="0" xr:uid="{28EAF8C7-F361-7B4A-983B-19A1D1C30C81}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -213,7 +213,7 @@
     impute 2 (Absent) if blank </t>
       </text>
     </comment>
-    <comment ref="E67" authorId="18" shapeId="0" xr:uid="{84CDE223-C27A-5D4D-90A3-3E5C1556727F}">
+    <comment ref="E68" authorId="18" shapeId="0" xr:uid="{84CDE223-C27A-5D4D-90A3-3E5C1556727F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -221,7 +221,7 @@
     impute 2 (No)</t>
       </text>
     </comment>
-    <comment ref="E68" authorId="19" shapeId="0" xr:uid="{4A341A6C-4C81-3543-82D1-C3658EBB86D4}">
+    <comment ref="E69" authorId="19" shapeId="0" xr:uid="{4A341A6C-4C81-3543-82D1-C3658EBB86D4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -229,7 +229,7 @@
     impute 2 (No)</t>
       </text>
     </comment>
-    <comment ref="E69" authorId="20" shapeId="0" xr:uid="{8BC0AFD8-E432-0A42-8EE8-5E4F5EC4EF1F}">
+    <comment ref="E70" authorId="20" shapeId="0" xr:uid="{8BC0AFD8-E432-0A42-8EE8-5E4F5EC4EF1F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -237,7 +237,7 @@
     impute 0</t>
       </text>
     </comment>
-    <comment ref="E71" authorId="21" shapeId="0" xr:uid="{1A8ADDA9-74B9-2744-B702-EED25DE7FB1F}">
+    <comment ref="E72" authorId="21" shapeId="0" xr:uid="{1A8ADDA9-74B9-2744-B702-EED25DE7FB1F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -245,7 +245,7 @@
     use Mammogram if available, else PET if available, otherwise impute 0</t>
       </text>
     </comment>
-    <comment ref="E74" authorId="22" shapeId="0" xr:uid="{BA67BED7-5470-F54C-A9B3-98B15C32C383}">
+    <comment ref="E75" authorId="22" shapeId="0" xr:uid="{BA67BED7-5470-F54C-A9B3-98B15C32C383}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -254,7 +254,7 @@
 Order: use MRI, else use PET, else impute 0. "</t>
       </text>
     </comment>
-    <comment ref="A127" authorId="23" shapeId="0" xr:uid="{1E3217F0-059D-9B4A-891F-86093E663007}">
+    <comment ref="A128" authorId="23" shapeId="0" xr:uid="{1E3217F0-059D-9B4A-891F-86093E663007}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -267,7 +267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="485">
   <si>
     <t>Field</t>
   </si>
@@ -1147,9 +1147,6 @@
     <t>Axillary lymph node core biopsy or FNA</t>
   </si>
   <si>
-    <t>Metastatic carcinoma on axillary lymph node biopsy</t>
-  </si>
-  <si>
     <t>if val == 2:
   val = 0.5</t>
   </si>
@@ -1611,24 +1608,12 @@
     <t>Pre-operative Systemic Therapy (Radiation Therapy)</t>
   </si>
   <si>
-    <t>Initial diagnostic imaging modality (Mammography)</t>
-  </si>
-  <si>
-    <t>Initial diagnostic imaging modality (U/S)</t>
-  </si>
-  <si>
     <t>Initial diagnostic imaging modality (MRI)</t>
   </si>
   <si>
-    <t>Histological subtype (IDC)</t>
-  </si>
-  <si>
     <t>Histological subtype (ILC)</t>
   </si>
   <si>
-    <t>Histological subtype (DCIS)</t>
-  </si>
-  <si>
     <t>Histological subtype (LCIS)</t>
   </si>
   <si>
@@ -1642,9 +1627,6 @@
   </si>
   <si>
     <t>Surgical Indication (Completion mast after after BCS w +ve margins)</t>
-  </si>
-  <si>
-    <t>Surgical Indication (Recurrent cancer)</t>
   </si>
   <si>
     <t>Surgical Indication (Second primary)</t>
@@ -1722,25 +1704,49 @@
     <t>Recommendation of PMRT</t>
   </si>
   <si>
-    <t>Presence of prominent, palpable, abnormal LN, or lymphadenopathy</t>
-  </si>
-  <si>
-    <t>Pre-operative breast biopsy type</t>
-  </si>
-  <si>
     <t>Whether histology was invasive (IDC, ILC, invasive mucinous, papillary)</t>
   </si>
   <si>
-    <t>Surgical Indication (Primary treatment)</t>
-  </si>
-  <si>
-    <t>The max size of tumor in mm (across ultrasound, mammography, and PET)</t>
-  </si>
-  <si>
-    <t>The largest abnormal LN size among pre-op LN sizes in mm (measured across modalities. Enter "0" if you chose "No abnormal LN" above.)</t>
-  </si>
-  <si>
     <t>Patient's age at imaging diagnosis in years</t>
+  </si>
+  <si>
+    <t>PRE_tumor_location_is_uiq</t>
+  </si>
+  <si>
+    <t>Whether the tumor is located in the upper-inner quadrant</t>
+  </si>
+  <si>
+    <t>Presence of metastatic carcinoma on axillary lymph node biopsy</t>
+  </si>
+  <si>
+    <t>Histology subtype is DCIS</t>
+  </si>
+  <si>
+    <t>Histology subtype is IDC</t>
+  </si>
+  <si>
+    <t>Presence of pre-operative suspicious/palpable lymph node or lymphadenopathy</t>
+  </si>
+  <si>
+    <t>Maximum dimension/size of pre-operative tumor</t>
+  </si>
+  <si>
+    <t>Maximum size of pre-operative suspicious lymph node</t>
+  </si>
+  <si>
+    <t>Initial diagnostic imaging modality is ultrasound</t>
+  </si>
+  <si>
+    <t>Pre-operative biopsy method</t>
+  </si>
+  <si>
+    <t>Surgical indication – primary treatment</t>
+  </si>
+  <si>
+    <t>Initial diagnostic imaging modality is mammography</t>
+  </si>
+  <si>
+    <t>Surgical indication – recurrent cancer</t>
   </si>
 </sst>
 </file>
@@ -1750,7 +1756,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1786,6 +1792,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="60">
@@ -2144,7 +2156,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -2152,11 +2164,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2225,6 +2252,10 @@
     <xf numFmtId="0" fontId="0" fillId="58" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="59" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="59" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2258,7 +2289,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2546,7 +2577,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2554,82 +2585,82 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D2" dT="2022-04-05T15:43:19.47" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{E88C6DA9-1AC2-0947-AA4C-0A0AE69DB287}">
+  <threadedComment ref="D3" dT="2022-04-05T15:43:19.47" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{E88C6DA9-1AC2-0947-AA4C-0A0AE69DB287}">
     <text>replace unknown (3) with missing, so that we can impute</text>
   </threadedComment>
-  <threadedComment ref="E3" dT="2022-04-07T01:22:20.36" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{0851E83E-F569-CC48-8979-68324726D851}">
+  <threadedComment ref="E4" dT="2022-04-07T01:22:20.36" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{0851E83E-F569-CC48-8979-68324726D851}">
     <text>Impute not palpable (0)</text>
   </threadedComment>
-  <threadedComment ref="A5" dT="2022-04-07T02:47:29.46" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{90142F8C-850A-2045-B460-594C957F7CEE}">
+  <threadedComment ref="A6" dT="2022-04-07T02:47:29.46" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{90142F8C-850A-2045-B460-594C957F7CEE}">
     <text>unexpected missingness; to be chart-reviewed</text>
   </threadedComment>
-  <threadedComment ref="J5" dT="2022-04-07T02:47:29.46" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{F44E1E05-68FC-C345-A086-9513C71E467A}">
+  <threadedComment ref="J6" dT="2022-04-07T02:47:29.46" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{F44E1E05-68FC-C345-A086-9513C71E467A}">
     <text>unexpected missingness; to be chart-reviewed</text>
   </threadedComment>
-  <threadedComment ref="E8" dT="2022-04-07T02:39:49.83" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{4E0ABAC6-E2DE-4D45-B44A-4E24BE55D192}">
+  <threadedComment ref="E9" dT="2022-04-07T02:39:49.83" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{4E0ABAC6-E2DE-4D45-B44A-4E24BE55D192}">
     <text>impute 0 if blank</text>
   </threadedComment>
-  <threadedComment ref="E9" dT="2022-04-07T01:14:47.45" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{5701CC43-81B2-5C4D-9C08-77ACBE9D2AB9}">
+  <threadedComment ref="E10" dT="2022-04-07T01:14:47.45" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{5701CC43-81B2-5C4D-9C08-77ACBE9D2AB9}">
     <text xml:space="preserve">TODO: Impute using Random Forest (H2O) trained on Post-op
 </text>
   </threadedComment>
-  <threadedComment ref="E9" dT="2022-04-07T01:16:37.12" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{80BCE8F6-75F3-564A-BE49-F052B6F4C793}" parentId="{5701CC43-81B2-5C4D-9C08-77ACBE9D2AB9}">
+  <threadedComment ref="E10" dT="2022-04-07T01:16:37.12" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{80BCE8F6-75F3-564A-BE49-F052B6F4C793}" parentId="{5701CC43-81B2-5C4D-9C08-77ACBE9D2AB9}">
     <text>TODO: Choose larger among img_size and tumor_size_mm</text>
   </threadedComment>
-  <threadedComment ref="D10" dT="2022-04-07T01:26:59.24" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{BE8AC716-1D1C-B642-BED8-C425D517B077}">
+  <threadedComment ref="D11" dT="2022-04-07T01:26:59.24" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{BE8AC716-1D1C-B642-BED8-C425D517B077}">
     <text>replace not mentioned with no</text>
   </threadedComment>
-  <threadedComment ref="E10" dT="2022-04-07T01:25:44.75" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{EEB800EB-04A9-0E4C-89C5-508F14B60227}">
+  <threadedComment ref="E11" dT="2022-04-07T01:25:44.75" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{EEB800EB-04A9-0E4C-89C5-508F14B60227}">
     <text>if blank, impute 2 (No). Replace 3 by 2.</text>
   </threadedComment>
-  <threadedComment ref="E11" dT="2022-04-07T01:22:54.01" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{98281554-B8B9-5C4C-8250-32226D76D614}">
+  <threadedComment ref="E12" dT="2022-04-07T01:22:54.01" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{98281554-B8B9-5C4C-8250-32226D76D614}">
     <text>TODO: Construct a new column with img_size, take the more authoritative measurement</text>
   </threadedComment>
-  <threadedComment ref="E13" dT="2022-04-07T01:36:13.47" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{4031F437-0C18-9A40-A568-C9BC83920B49}">
+  <threadedComment ref="E14" dT="2022-04-07T01:36:13.47" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{4031F437-0C18-9A40-A568-C9BC83920B49}">
     <text xml:space="preserve">TODO: Construct a new column with lymph_node_max_size_mm </text>
   </threadedComment>
-  <threadedComment ref="E14" dT="2022-04-07T01:27:54.33" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{D7EDEE7B-587E-D848-8C5D-279BA8E53A36}">
+  <threadedComment ref="E15" dT="2022-04-07T01:27:54.33" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{D7EDEE7B-587E-D848-8C5D-279BA8E53A36}">
     <text>drop variable because ultrasound is better?</text>
   </threadedComment>
-  <threadedComment ref="E15" dT="2022-04-07T01:37:09.66" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{E1553B31-F607-BE4A-81A5-7BBE8308D7DF}">
+  <threadedComment ref="E16" dT="2022-04-07T01:37:09.66" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{E1553B31-F607-BE4A-81A5-7BBE8308D7DF}">
     <text>impute 0 if blank, convert to binary variable</text>
   </threadedComment>
-  <threadedComment ref="E39" dT="2022-04-07T02:45:37.51" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{04ADA115-B14D-1848-B5AE-2A1C3D5ED21A}">
+  <threadedComment ref="E40" dT="2022-04-07T02:45:37.51" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{04ADA115-B14D-1848-B5AE-2A1C3D5ED21A}">
     <text>TODO: group 2 and 3 together; 4 and 5 together</text>
   </threadedComment>
-  <threadedComment ref="E54" dT="2022-04-07T01:10:28.90" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{707F85C7-4A70-8445-AD41-E181BA97C713}">
+  <threadedComment ref="E55" dT="2022-04-07T01:10:28.90" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{707F85C7-4A70-8445-AD41-E181BA97C713}">
     <text>TODO: "Construct a new column: Age at diagnosis or surgery
 Impute: Jan 2020"</text>
   </threadedComment>
-  <threadedComment ref="E62" dT="2022-04-07T01:25:55.07" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{35A6CD70-95AF-CA4E-AD09-29213DDCD3C0}">
+  <threadedComment ref="E63" dT="2022-04-07T01:25:55.07" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{35A6CD70-95AF-CA4E-AD09-29213DDCD3C0}">
     <text>impute 0 if blank</text>
   </threadedComment>
-  <threadedComment ref="E64" dT="2022-04-07T01:35:10.24" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{E7E014ED-CA32-CF4B-B7EA-09A950207112}">
+  <threadedComment ref="E65" dT="2022-04-07T01:35:10.24" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{E7E014ED-CA32-CF4B-B7EA-09A950207112}">
     <text>ie don’t manually impute</text>
   </threadedComment>
-  <threadedComment ref="E65" dT="2022-04-07T01:26:15.80" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{CFBAAC2D-21C1-684D-9816-483DFFD98BA2}">
+  <threadedComment ref="E66" dT="2022-04-07T01:26:15.80" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{CFBAAC2D-21C1-684D-9816-483DFFD98BA2}">
     <text>impute 1 (most are unifocal), replace 0 with 1.</text>
   </threadedComment>
-  <threadedComment ref="E66" dT="2022-04-07T01:32:15.54" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{28EAF8C7-F361-7B4A-983B-19A1D1C30C81}">
+  <threadedComment ref="E67" dT="2022-04-07T01:32:15.54" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{28EAF8C7-F361-7B4A-983B-19A1D1C30C81}">
     <text xml:space="preserve">impute 2 (Absent) if blank </text>
   </threadedComment>
-  <threadedComment ref="E67" dT="2022-04-07T01:31:33.71" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{84CDE223-C27A-5D4D-90A3-3E5C1556727F}">
+  <threadedComment ref="E68" dT="2022-04-07T01:31:33.71" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{84CDE223-C27A-5D4D-90A3-3E5C1556727F}">
     <text>impute 2 (No)</text>
   </threadedComment>
-  <threadedComment ref="E68" dT="2022-04-07T01:31:37.20" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{4A341A6C-4C81-3543-82D1-C3658EBB86D4}">
+  <threadedComment ref="E69" dT="2022-04-07T01:31:37.20" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{4A341A6C-4C81-3543-82D1-C3658EBB86D4}">
     <text>impute 2 (No)</text>
   </threadedComment>
-  <threadedComment ref="E69" dT="2022-04-07T01:32:04.81" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{8BC0AFD8-E432-0A42-8EE8-5E4F5EC4EF1F}">
+  <threadedComment ref="E70" dT="2022-04-07T01:32:04.81" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{8BC0AFD8-E432-0A42-8EE8-5E4F5EC4EF1F}">
     <text>impute 0</text>
   </threadedComment>
-  <threadedComment ref="E71" dT="2022-04-07T01:22:01.71" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{1A8ADDA9-74B9-2744-B702-EED25DE7FB1F}">
+  <threadedComment ref="E72" dT="2022-04-07T01:22:01.71" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{1A8ADDA9-74B9-2744-B702-EED25DE7FB1F}">
     <text>use Mammogram if available, else PET if available, otherwise impute 0</text>
   </threadedComment>
-  <threadedComment ref="E74" dT="2022-04-07T01:36:36.87" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{BA67BED7-5470-F54C-A9B3-98B15C32C383}">
+  <threadedComment ref="E75" dT="2022-04-07T01:36:36.87" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{BA67BED7-5470-F54C-A9B3-98B15C32C383}">
     <text>"Group with MRI (internal_mammary_lymphaden), PET. 
 Order: use MRI, else use PET, else impute 0. "</text>
   </threadedComment>
-  <threadedComment ref="A127" dT="2022-09-06T17:57:27.04" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{1E3217F0-059D-9B4A-891F-86093E663007}">
+  <threadedComment ref="A128" dT="2022-09-06T17:57:27.04" personId="{56AAE3F1-586C-3A49-8F14-F5F9AD03C363}" id="{1E3217F0-059D-9B4A-891F-86093E663007}">
     <text>Unsure whether to remove these?</text>
   </threadedComment>
 </ThreadedComments>
@@ -2638,11 +2669,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05D32D06-7DAE-3944-9C50-40C3579C6515}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J145"/>
+  <dimension ref="A1:J147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H126" sqref="H126"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="113" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2665,7 +2696,7 @@
         <v>167</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>236</v>
@@ -2683,402 +2714,394 @@
         <v>84</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2E-3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C2" s="5">
-        <v>2E-3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="F2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="F3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H3" t="s">
         <v>220</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C3" s="11">
+      <c r="B4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="11">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>235</v>
       </c>
-      <c r="F3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="F4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" t="s">
         <v>233</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:10" ht="82" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>44</v>
       </c>
-      <c r="B4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C4" s="33">
+      <c r="B5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" s="33">
         <v>6.2E-2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="E4" t="s">
-        <v>307</v>
-      </c>
-      <c r="F4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="H4" t="s">
-        <v>284</v>
-      </c>
-      <c r="J4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="102" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C5" s="33">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>305</v>
+      <c r="E5" t="s">
+        <v>306</v>
       </c>
       <c r="F5" t="s">
         <v>82</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>275</v>
+        <v>412</v>
       </c>
       <c r="H5" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="J5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
         <v>168</v>
       </c>
-      <c r="C6" s="38">
-        <v>0.153</v>
+      <c r="C6" s="33">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="E6" t="s">
-        <v>307</v>
+        <v>276</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>304</v>
       </c>
       <c r="F6" t="s">
         <v>82</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>413</v>
+        <v>275</v>
       </c>
       <c r="H6" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="J6" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
         <v>168</v>
       </c>
-      <c r="C7" s="39">
-        <v>0.155</v>
+      <c r="C7" s="38">
+        <v>0.153</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>287</v>
       </c>
       <c r="E7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F7" t="s">
         <v>82</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H7" t="s">
+        <v>285</v>
+      </c>
+      <c r="J7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" s="39">
+        <v>0.155</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="E8" t="s">
+        <v>306</v>
+      </c>
+      <c r="F8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="H8" t="s">
         <v>286</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J8" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C8" s="37">
-        <v>0.17299999999999999</v>
-      </c>
-      <c r="E8" t="s">
-        <v>235</v>
-      </c>
-      <c r="F8" t="s">
-        <v>80</v>
-      </c>
-      <c r="G8" t="s">
-        <v>301</v>
-      </c>
-      <c r="H8" t="s">
-        <v>283</v>
-      </c>
-      <c r="J8" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="37">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="E9" t="s">
+        <v>235</v>
+      </c>
+      <c r="F9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" t="s">
+        <v>300</v>
+      </c>
+      <c r="H9" t="s">
+        <v>283</v>
+      </c>
+      <c r="J9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
-        <v>168</v>
-      </c>
-      <c r="C9" s="14">
+      <c r="B10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="14">
         <v>0.245</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>85</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>81</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>240</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J10" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
-        <v>168</v>
-      </c>
-      <c r="C10" s="22">
+      <c r="B11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="22">
         <v>0.27</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>258</v>
       </c>
-      <c r="F10" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="F11" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H11" t="s">
         <v>253</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J11" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
-        <v>168</v>
-      </c>
-      <c r="C11" s="19">
+      <c r="B12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12" s="19">
         <v>0.55500000000000005</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>86</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>81</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H12" t="s">
         <v>250</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="64" t="s">
+    <row r="13" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="B12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C12" s="41">
+      <c r="B13" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="41">
         <v>0.66200000000000003</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D13" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E13" t="s">
         <v>235</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>82</v>
       </c>
-      <c r="G12" t="s">
-        <v>414</v>
-      </c>
-      <c r="H12" t="s">
-        <v>290</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="G13" t="s">
+        <v>413</v>
+      </c>
+      <c r="H13" s="66" t="s">
+        <v>474</v>
+      </c>
+      <c r="J13" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>168</v>
-      </c>
-      <c r="C13" s="29">
-        <v>0.95199999999999996</v>
-      </c>
-      <c r="E13" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" t="s">
-        <v>81</v>
-      </c>
-      <c r="H13" t="s">
-        <v>265</v>
-      </c>
-      <c r="J13" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
         <v>168</v>
       </c>
-      <c r="C14" s="23">
-        <v>0.98499999999999999</v>
+      <c r="C14" s="29">
+        <v>0.95199999999999996</v>
       </c>
       <c r="E14" t="s">
-        <v>306</v>
+        <v>87</v>
       </c>
       <c r="F14" t="s">
         <v>81</v>
       </c>
       <c r="H14" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="J14" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
         <v>168</v>
       </c>
-      <c r="C15" s="30">
-        <v>0.99199999999999999</v>
+      <c r="C15" s="23">
+        <v>0.98499999999999999</v>
       </c>
       <c r="E15" t="s">
-        <v>235</v>
+        <v>305</v>
       </c>
       <c r="F15" t="s">
         <v>81</v>
       </c>
       <c r="H15" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="J15" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
         <v>168</v>
       </c>
-      <c r="C16" s="5">
-        <v>0</v>
+      <c r="C16" s="30">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="E16" t="s">
+        <v>235</v>
       </c>
       <c r="F16" t="s">
-        <v>273</v>
+        <v>81</v>
       </c>
       <c r="H16" t="s">
-        <v>218</v>
+        <v>267</v>
       </c>
       <c r="J16" t="s">
-        <v>88</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
         <v>168</v>
@@ -3087,18 +3110,18 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>79</v>
+        <v>273</v>
       </c>
       <c r="H17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>373</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
         <v>168</v>
@@ -3107,24 +3130,18 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>80</v>
-      </c>
-      <c r="G18" t="s">
-        <v>262</v>
+        <v>79</v>
       </c>
       <c r="H18" t="s">
-        <v>429</v>
-      </c>
-      <c r="I18" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="J18" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B19" t="s">
         <v>168</v>
@@ -3139,15 +3156,18 @@
         <v>262</v>
       </c>
       <c r="H19" t="s">
-        <v>430</v>
+        <v>428</v>
+      </c>
+      <c r="I19" t="s">
+        <v>223</v>
       </c>
       <c r="J19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B20" t="s">
         <v>168</v>
@@ -3162,15 +3182,15 @@
         <v>262</v>
       </c>
       <c r="H20" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="J20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B21" t="s">
         <v>168</v>
@@ -3185,15 +3205,15 @@
         <v>262</v>
       </c>
       <c r="H21" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="J21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B22" t="s">
         <v>168</v>
@@ -3208,15 +3228,15 @@
         <v>262</v>
       </c>
       <c r="H22" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="J22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B23" t="s">
         <v>168</v>
@@ -3231,15 +3251,15 @@
         <v>262</v>
       </c>
       <c r="H23" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="J23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B24" t="s">
         <v>168</v>
@@ -3254,15 +3274,15 @@
         <v>262</v>
       </c>
       <c r="H24" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="J24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>368</v>
+        <v>378</v>
       </c>
       <c r="B25" t="s">
         <v>168</v>
@@ -3277,18 +3297,15 @@
         <v>262</v>
       </c>
       <c r="H25" t="s">
-        <v>436</v>
-      </c>
-      <c r="I25" t="s">
-        <v>224</v>
+        <v>434</v>
       </c>
       <c r="J25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B26" t="s">
         <v>168</v>
@@ -3303,15 +3320,18 @@
         <v>262</v>
       </c>
       <c r="H26" t="s">
-        <v>437</v>
+        <v>435</v>
+      </c>
+      <c r="I26" t="s">
+        <v>224</v>
       </c>
       <c r="J26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B27" t="s">
         <v>168</v>
@@ -3326,15 +3346,15 @@
         <v>262</v>
       </c>
       <c r="H27" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="J27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="64" t="s">
-        <v>371</v>
+      <c r="A28" t="s">
+        <v>369</v>
       </c>
       <c r="B28" t="s">
         <v>168</v>
@@ -3349,15 +3369,15 @@
         <v>262</v>
       </c>
       <c r="H28" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="J28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>372</v>
+      <c r="A29" s="64" t="s">
+        <v>370</v>
       </c>
       <c r="B29" t="s">
         <v>168</v>
@@ -3365,9 +3385,6 @@
       <c r="C29" s="5">
         <v>0</v>
       </c>
-      <c r="D29" t="s">
-        <v>225</v>
-      </c>
       <c r="F29" t="s">
         <v>80</v>
       </c>
@@ -3375,15 +3392,15 @@
         <v>262</v>
       </c>
       <c r="H29" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="J29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>397</v>
+        <v>371</v>
       </c>
       <c r="B30" t="s">
         <v>168</v>
@@ -3391,6 +3408,9 @@
       <c r="C30" s="5">
         <v>0</v>
       </c>
+      <c r="D30" t="s">
+        <v>225</v>
+      </c>
       <c r="F30" t="s">
         <v>80</v>
       </c>
@@ -3398,18 +3418,15 @@
         <v>262</v>
       </c>
       <c r="H30" t="s">
-        <v>441</v>
-      </c>
-      <c r="I30" t="s">
-        <v>234</v>
+        <v>439</v>
       </c>
       <c r="J30" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>366</v>
+        <v>396</v>
       </c>
       <c r="B31" t="s">
         <v>168</v>
@@ -3424,15 +3441,18 @@
         <v>262</v>
       </c>
       <c r="H31" t="s">
-        <v>442</v>
+        <v>483</v>
+      </c>
+      <c r="I31" t="s">
+        <v>234</v>
       </c>
       <c r="J31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B32" t="s">
         <v>168</v>
@@ -3447,15 +3467,15 @@
         <v>262</v>
       </c>
       <c r="H32" t="s">
-        <v>443</v>
+        <v>480</v>
       </c>
       <c r="J32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="B33" t="s">
         <v>168</v>
@@ -3470,18 +3490,15 @@
         <v>262</v>
       </c>
       <c r="H33" t="s">
-        <v>444</v>
-      </c>
-      <c r="I33" t="s">
-        <v>271</v>
+        <v>440</v>
       </c>
       <c r="J33" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B34" t="s">
         <v>168</v>
@@ -3495,16 +3512,19 @@
       <c r="G34" t="s">
         <v>262</v>
       </c>
-      <c r="H34" t="s">
-        <v>445</v>
+      <c r="H34" s="66" t="s">
+        <v>476</v>
+      </c>
+      <c r="I34" t="s">
+        <v>271</v>
       </c>
       <c r="J34" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="74" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B35" t="s">
         <v>168</v>
@@ -3519,15 +3539,15 @@
         <v>262</v>
       </c>
       <c r="H35" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="J35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B36" t="s">
         <v>168</v>
@@ -3541,16 +3561,16 @@
       <c r="G36" t="s">
         <v>262</v>
       </c>
-      <c r="H36" t="s">
-        <v>447</v>
+      <c r="H36" s="66" t="s">
+        <v>475</v>
       </c>
       <c r="J36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B37" t="s">
         <v>168</v>
@@ -3565,15 +3585,15 @@
         <v>262</v>
       </c>
       <c r="H37" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="J37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B38" t="s">
         <v>168</v>
@@ -3588,15 +3608,15 @@
         <v>262</v>
       </c>
       <c r="H38" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="J38" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>400</v>
+        <v>364</v>
       </c>
       <c r="B39" t="s">
         <v>168</v>
@@ -3604,28 +3624,22 @@
       <c r="C39" s="5">
         <v>0</v>
       </c>
-      <c r="E39" t="s">
-        <v>297</v>
-      </c>
       <c r="F39" t="s">
         <v>80</v>
       </c>
       <c r="G39" t="s">
         <v>262</v>
       </c>
-      <c r="H39" s="3" t="s">
-        <v>479</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>292</v>
+      <c r="H39" t="s">
+        <v>444</v>
       </c>
       <c r="J39" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B40" t="s">
         <v>168</v>
@@ -3633,6 +3647,9 @@
       <c r="C40" s="5">
         <v>0</v>
       </c>
+      <c r="E40" t="s">
+        <v>296</v>
+      </c>
       <c r="F40" t="s">
         <v>80</v>
       </c>
@@ -3640,15 +3657,18 @@
         <v>262</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>450</v>
+        <v>482</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>291</v>
       </c>
       <c r="J40" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B41" t="s">
         <v>168</v>
@@ -3663,15 +3683,15 @@
         <v>262</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="J41" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="65" t="s">
-        <v>398</v>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>401</v>
       </c>
       <c r="B42" t="s">
         <v>168</v>
@@ -3686,15 +3706,15 @@
         <v>262</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="J42" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>399</v>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="65" t="s">
+        <v>397</v>
       </c>
       <c r="B43" t="s">
         <v>168</v>
@@ -3708,26 +3728,23 @@
       <c r="G43" t="s">
         <v>262</v>
       </c>
-      <c r="H43" s="3" t="s">
-        <v>453</v>
+      <c r="H43" s="67" t="s">
+        <v>484</v>
       </c>
       <c r="J43" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A44" s="64" t="s">
-        <v>473</v>
-      </c>
-      <c r="B44" s="64" t="s">
-        <v>170</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>398</v>
+      </c>
+      <c r="B44" t="s">
+        <v>168</v>
       </c>
       <c r="C44" s="5">
         <v>0</v>
       </c>
-      <c r="E44" t="s">
-        <v>235</v>
-      </c>
       <c r="F44" t="s">
         <v>80</v>
       </c>
@@ -3735,18 +3752,15 @@
         <v>262</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>300</v>
+        <v>447</v>
       </c>
       <c r="J44" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="64" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="B45" s="64" t="s">
         <v>170</v>
@@ -3754,6 +3768,9 @@
       <c r="C45" s="5">
         <v>0</v>
       </c>
+      <c r="E45" t="s">
+        <v>235</v>
+      </c>
       <c r="F45" t="s">
         <v>80</v>
       </c>
@@ -3761,15 +3778,18 @@
         <v>262</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>455</v>
+        <v>448</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>299</v>
       </c>
       <c r="J45" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="64" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="B46" s="64" t="s">
         <v>170</v>
@@ -3784,132 +3804,132 @@
         <v>262</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="J46" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="64" t="s">
+        <v>465</v>
+      </c>
+      <c r="B47" s="64" t="s">
+        <v>170</v>
+      </c>
+      <c r="C47" s="5">
+        <v>0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>80</v>
+      </c>
+      <c r="G47" t="s">
+        <v>262</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="J47" t="s">
         <v>166</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" t="s">
-        <v>168</v>
-      </c>
-      <c r="C47" s="5">
-        <v>2E-3</v>
-      </c>
-      <c r="F47" t="s">
-        <v>80</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="H47" t="s">
-        <v>226</v>
-      </c>
-      <c r="J47" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
+        <v>168</v>
+      </c>
+      <c r="C48" s="5">
+        <v>2E-3</v>
+      </c>
+      <c r="F48" t="s">
+        <v>80</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="H48" t="s">
+        <v>226</v>
+      </c>
+      <c r="J48" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>50</v>
       </c>
-      <c r="B48" t="s">
-        <v>168</v>
-      </c>
-      <c r="C48" s="5">
+      <c r="B49" t="s">
+        <v>168</v>
+      </c>
+      <c r="C49" s="5">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F48" t="s">
-        <v>80</v>
-      </c>
-      <c r="G48" s="3" t="s">
+      <c r="F49" t="s">
+        <v>80</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="I49" s="3"/>
+      <c r="J49" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" t="s">
+        <v>168</v>
+      </c>
+      <c r="C50" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="F50" t="s">
+        <v>80</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="H50" t="s">
+        <v>298</v>
+      </c>
+      <c r="J50" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>168</v>
+      </c>
+      <c r="C51" s="6">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E51" s="63" t="s">
+        <v>295</v>
+      </c>
+      <c r="F51" t="s">
+        <v>79</v>
+      </c>
+      <c r="H51" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="H48" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="I48" s="3"/>
-      <c r="J48" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" t="s">
-        <v>168</v>
-      </c>
-      <c r="C49" s="6">
-        <v>0.01</v>
-      </c>
-      <c r="F49" t="s">
-        <v>80</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H49" t="s">
-        <v>299</v>
-      </c>
-      <c r="J49" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" t="s">
-        <v>168</v>
-      </c>
-      <c r="C50" s="6">
-        <v>1.2E-2</v>
-      </c>
-      <c r="E50" s="63" t="s">
-        <v>296</v>
-      </c>
-      <c r="F50" t="s">
-        <v>79</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="I50" s="3"/>
-      <c r="J50" t="s">
+      <c r="I51" s="3"/>
+      <c r="J51" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>5</v>
-      </c>
-      <c r="B51" t="s">
-        <v>168</v>
-      </c>
-      <c r="C51" s="6">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="F51" t="s">
-        <v>80</v>
-      </c>
-      <c r="G51" t="s">
-        <v>262</v>
-      </c>
-      <c r="H51" t="s">
-        <v>222</v>
-      </c>
-      <c r="J51" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>35</v>
       </c>
       <c r="B52" t="s">
         <v>168</v>
@@ -3920,365 +3940,362 @@
       <c r="F52" t="s">
         <v>80</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="G52" t="s">
+        <v>262</v>
+      </c>
+      <c r="H52" t="s">
+        <v>222</v>
+      </c>
+      <c r="J52" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" t="s">
+        <v>168</v>
+      </c>
+      <c r="C53" s="6">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="F53" t="s">
+        <v>80</v>
+      </c>
+      <c r="G53" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="H52" t="s">
-        <v>477</v>
-      </c>
-      <c r="J52" t="s">
+      <c r="H53" t="s">
+        <v>481</v>
+      </c>
+      <c r="J53" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>11</v>
-      </c>
-      <c r="B53" t="s">
-        <v>168</v>
-      </c>
-      <c r="C53" s="10">
-        <v>0.02</v>
-      </c>
-      <c r="F53" t="s">
-        <v>80</v>
-      </c>
-      <c r="H53" t="s">
-        <v>232</v>
-      </c>
-      <c r="J53" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
         <v>168</v>
       </c>
-      <c r="C54" s="12">
-        <v>2.3E-2</v>
+      <c r="C54" s="10">
+        <v>0.02</v>
       </c>
       <c r="F54" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H54" t="s">
-        <v>279</v>
+        <v>232</v>
       </c>
       <c r="J54" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B55" t="s">
         <v>168</v>
       </c>
-      <c r="C55" s="11">
-        <v>4.4999999999999998E-2</v>
+      <c r="C55" s="12">
+        <v>2.3E-2</v>
       </c>
       <c r="F55" t="s">
         <v>79</v>
       </c>
       <c r="H55" t="s">
+        <v>279</v>
+      </c>
+      <c r="J55" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>34</v>
+      </c>
+      <c r="B56" t="s">
+        <v>168</v>
+      </c>
+      <c r="C56" s="11">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F56" t="s">
+        <v>79</v>
+      </c>
+      <c r="H56" t="s">
         <v>268</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J56" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="57" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>47</v>
       </c>
-      <c r="B56" t="s">
-        <v>168</v>
-      </c>
-      <c r="C56" s="33">
+      <c r="B57" t="s">
+        <v>168</v>
+      </c>
+      <c r="C57" s="33">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D57" s="3" t="s">
         <v>287</v>
-      </c>
-      <c r="F56" t="s">
-        <v>82</v>
-      </c>
-      <c r="G56" t="s">
-        <v>247</v>
-      </c>
-      <c r="H56" t="s">
-        <v>288</v>
-      </c>
-      <c r="J56" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>48</v>
-      </c>
-      <c r="B57" t="s">
-        <v>168</v>
-      </c>
-      <c r="C57" s="40">
-        <v>0.08</v>
-      </c>
-      <c r="E57" t="s">
-        <v>235</v>
       </c>
       <c r="F57" t="s">
         <v>82</v>
       </c>
-      <c r="G57" s="3" t="s">
+      <c r="G57" t="s">
+        <v>247</v>
+      </c>
+      <c r="H57" t="s">
+        <v>288</v>
+      </c>
+      <c r="J57" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>48</v>
+      </c>
+      <c r="B58" t="s">
+        <v>168</v>
+      </c>
+      <c r="C58" s="40">
+        <v>0.08</v>
+      </c>
+      <c r="E58" t="s">
+        <v>235</v>
+      </c>
+      <c r="F58" t="s">
+        <v>82</v>
+      </c>
+      <c r="G58" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="H57" t="s">
+      <c r="H58" t="s">
         <v>289</v>
       </c>
-      <c r="J57" t="s">
+      <c r="J58" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>21</v>
       </c>
-      <c r="B58" t="s">
-        <v>168</v>
-      </c>
-      <c r="C58" s="20">
+      <c r="B59" t="s">
+        <v>168</v>
+      </c>
+      <c r="C59" s="20">
         <v>0.19800000000000001</v>
       </c>
-      <c r="F58" t="s">
-        <v>80</v>
-      </c>
-      <c r="H58" t="s">
+      <c r="F59" t="s">
+        <v>80</v>
+      </c>
+      <c r="H59" t="s">
         <v>251</v>
       </c>
-      <c r="J58" t="s">
+      <c r="J59" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="60" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>18</v>
       </c>
-      <c r="B59" t="s">
-        <v>168</v>
-      </c>
-      <c r="C59" s="17">
+      <c r="B60" t="s">
+        <v>168</v>
+      </c>
+      <c r="C60" s="17">
         <v>0.24199999999999999</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="D60" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="E60" t="s">
         <v>235</v>
       </c>
-      <c r="F59" t="s">
-        <v>80</v>
-      </c>
-      <c r="G59" s="3" t="s">
+      <c r="F60" t="s">
+        <v>80</v>
+      </c>
+      <c r="G60" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H60" t="s">
         <v>246</v>
       </c>
-      <c r="J59" t="s">
+      <c r="J60" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>36</v>
-      </c>
-      <c r="B60" t="s">
-        <v>168</v>
-      </c>
-      <c r="C60" s="31">
-        <v>0.48</v>
-      </c>
-      <c r="F60" t="s">
-        <v>80</v>
-      </c>
-      <c r="H60" t="s">
-        <v>270</v>
-      </c>
-      <c r="J60" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B61" t="s">
         <v>168</v>
       </c>
-      <c r="C61" s="8">
-        <v>0.60699999999999998</v>
+      <c r="C61" s="31">
+        <v>0.48</v>
       </c>
       <c r="F61" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H61" t="s">
-        <v>229</v>
+        <v>270</v>
       </c>
       <c r="J61" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B62" t="s">
         <v>168</v>
       </c>
-      <c r="C62" s="21">
-        <v>0.61</v>
-      </c>
-      <c r="E62" t="s">
-        <v>235</v>
+      <c r="C62" s="8">
+        <v>0.60699999999999998</v>
       </c>
       <c r="F62" t="s">
         <v>81</v>
       </c>
       <c r="H62" t="s">
-        <v>252</v>
+        <v>229</v>
       </c>
       <c r="J62" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B63" t="s">
         <v>168</v>
       </c>
-      <c r="C63" s="7">
-        <v>0.63800000000000001</v>
+      <c r="C63" s="21">
+        <v>0.61</v>
+      </c>
+      <c r="E63" t="s">
+        <v>235</v>
       </c>
       <c r="F63" t="s">
         <v>81</v>
       </c>
       <c r="H63" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
       <c r="J63" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B64" t="s">
         <v>168</v>
       </c>
-      <c r="C64" s="13">
-        <v>0.69799999999999995</v>
-      </c>
-      <c r="E64" t="s">
-        <v>238</v>
+      <c r="C64" s="7">
+        <v>0.63800000000000001</v>
       </c>
       <c r="F64" t="s">
         <v>81</v>
       </c>
-      <c r="H64" s="60" t="s">
+      <c r="H64" t="s">
+        <v>228</v>
+      </c>
+      <c r="J64" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65" t="s">
+        <v>168</v>
+      </c>
+      <c r="C65" s="13">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="E65" t="s">
+        <v>238</v>
+      </c>
+      <c r="F65" t="s">
+        <v>81</v>
+      </c>
+      <c r="H65" s="60" t="s">
         <v>239</v>
       </c>
-      <c r="I64" s="60"/>
-      <c r="J64" t="s">
+      <c r="I65" s="60"/>
+      <c r="J65" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="66" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>16</v>
       </c>
-      <c r="B65" t="s">
-        <v>168</v>
-      </c>
-      <c r="C65" s="15">
+      <c r="B66" t="s">
+        <v>168</v>
+      </c>
+      <c r="C66" s="15">
         <v>0.71699999999999997</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D66" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E66" t="s">
         <v>242</v>
       </c>
-      <c r="F65" t="s">
-        <v>309</v>
-      </c>
-      <c r="H65" t="s">
+      <c r="F66" t="s">
+        <v>308</v>
+      </c>
+      <c r="H66" t="s">
         <v>241</v>
       </c>
-      <c r="J65" t="s">
+      <c r="J66" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="67" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>25</v>
       </c>
-      <c r="B66" t="s">
-        <v>168</v>
-      </c>
-      <c r="C66" s="24">
+      <c r="B67" t="s">
+        <v>168</v>
+      </c>
+      <c r="C67" s="24">
         <v>0.76500000000000001</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E67" t="s">
         <v>258</v>
-      </c>
-      <c r="F66" t="s">
-        <v>82</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="H66" t="s">
-        <v>256</v>
-      </c>
-      <c r="J66" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>26</v>
-      </c>
-      <c r="B67" t="s">
-        <v>168</v>
-      </c>
-      <c r="C67" s="26">
-        <v>0.77</v>
-      </c>
-      <c r="E67" t="s">
-        <v>235</v>
       </c>
       <c r="F67" t="s">
         <v>82</v>
       </c>
-      <c r="G67" t="s">
-        <v>262</v>
+      <c r="G67" s="3" t="s">
+        <v>257</v>
       </c>
       <c r="H67" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="J67" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B68" t="s">
         <v>168</v>
@@ -4296,474 +4313,474 @@
         <v>262</v>
       </c>
       <c r="H68" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J68" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A69" s="60" t="s">
-        <v>302</v>
+      <c r="A69" t="s">
+        <v>27</v>
       </c>
       <c r="B69" t="s">
         <v>168</v>
       </c>
-      <c r="C69" s="25">
-        <v>0.78800000000000003</v>
+      <c r="C69" s="26">
+        <v>0.77</v>
       </c>
       <c r="E69" t="s">
         <v>235</v>
       </c>
       <c r="F69" t="s">
+        <v>82</v>
+      </c>
+      <c r="G69" t="s">
+        <v>262</v>
+      </c>
+      <c r="H69" t="s">
+        <v>261</v>
+      </c>
+      <c r="J69" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" s="60" t="s">
+        <v>301</v>
+      </c>
+      <c r="B70" t="s">
+        <v>168</v>
+      </c>
+      <c r="C70" s="25">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="E70" t="s">
+        <v>235</v>
+      </c>
+      <c r="F70" t="s">
         <v>81</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H70" t="s">
         <v>259</v>
       </c>
-      <c r="J69" s="60" t="s">
+      <c r="J70" s="60" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+    <row r="71" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>17</v>
       </c>
-      <c r="B70" t="s">
-        <v>168</v>
-      </c>
-      <c r="C70" s="16">
+      <c r="B71" t="s">
+        <v>168</v>
+      </c>
+      <c r="C71" s="16">
         <v>0.8</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E71" t="s">
         <v>238</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F71" t="s">
         <v>82</v>
       </c>
-      <c r="G70" s="3" t="s">
+      <c r="G71" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H71" t="s">
         <v>244</v>
       </c>
-      <c r="J70" t="s">
+      <c r="J71" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="170" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+    <row r="72" spans="1:10" ht="170" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>19</v>
       </c>
-      <c r="B71" t="s">
-        <v>168</v>
-      </c>
-      <c r="C71" s="18">
+      <c r="B72" t="s">
+        <v>168</v>
+      </c>
+      <c r="C72" s="18">
         <v>0.877</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="E72" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F72" t="s">
         <v>81</v>
       </c>
-      <c r="H71" t="s">
+      <c r="H72" t="s">
         <v>248</v>
       </c>
-      <c r="J71" t="s">
+      <c r="J72" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>40</v>
-      </c>
-      <c r="B72" t="s">
-        <v>168</v>
-      </c>
-      <c r="C72" s="34">
-        <v>0.91200000000000003</v>
-      </c>
-      <c r="F72" t="s">
-        <v>82</v>
-      </c>
-      <c r="G72" t="s">
-        <v>278</v>
-      </c>
-      <c r="H72" t="s">
-        <v>277</v>
-      </c>
-      <c r="J72" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B73" t="s">
         <v>168</v>
       </c>
-      <c r="C73" s="27">
-        <v>0.91800000000000004</v>
-      </c>
-      <c r="E73" t="s">
-        <v>235</v>
+      <c r="C73" s="34">
+        <v>0.91200000000000003</v>
       </c>
       <c r="F73" t="s">
         <v>82</v>
       </c>
       <c r="G73" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="H73" t="s">
-        <v>264</v>
+        <v>277</v>
       </c>
       <c r="J73" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B74" t="s">
         <v>168</v>
       </c>
       <c r="C74" s="27">
-        <v>0.92</v>
-      </c>
-      <c r="E74" s="3" t="s">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="E74" t="s">
         <v>235</v>
       </c>
       <c r="F74" t="s">
         <v>82</v>
       </c>
+      <c r="G74" t="s">
+        <v>262</v>
+      </c>
       <c r="H74" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J74" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B75" t="s">
         <v>168</v>
       </c>
       <c r="C75" s="27">
-        <v>0.92200000000000004</v>
-      </c>
-      <c r="E75" t="s">
-        <v>238</v>
+        <v>0.92</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>235</v>
       </c>
       <c r="F75" t="s">
         <v>82</v>
       </c>
-      <c r="G75" t="s">
-        <v>262</v>
-      </c>
       <c r="H75" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="J75" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B76" t="s">
         <v>168</v>
       </c>
-      <c r="C76" s="35">
-        <v>0.92500000000000004</v>
+      <c r="C76" s="27">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="E76" t="s">
+        <v>238</v>
       </c>
       <c r="F76" t="s">
-        <v>80</v>
+        <v>82</v>
+      </c>
+      <c r="G76" t="s">
+        <v>262</v>
       </c>
       <c r="H76" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="J76" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B77" t="s">
         <v>168</v>
       </c>
-      <c r="C77" s="28">
-        <v>0.94199999999999995</v>
-      </c>
-      <c r="E77" t="s">
-        <v>238</v>
+      <c r="C77" s="35">
+        <v>0.92500000000000004</v>
       </c>
       <c r="F77" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H77" t="s">
-        <v>463</v>
+        <v>280</v>
       </c>
       <c r="J77" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>29</v>
+      </c>
+      <c r="B78" t="s">
+        <v>168</v>
+      </c>
+      <c r="C78" s="28">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="E78" t="s">
+        <v>238</v>
+      </c>
+      <c r="F78" t="s">
+        <v>81</v>
+      </c>
+      <c r="H78" t="s">
+        <v>457</v>
+      </c>
+      <c r="J78" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>38</v>
       </c>
-      <c r="B78" t="s">
-        <v>168</v>
-      </c>
-      <c r="C78" s="32">
+      <c r="B79" t="s">
+        <v>168</v>
+      </c>
+      <c r="C79" s="32">
         <v>0.96299999999999997</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F79" t="s">
         <v>273</v>
       </c>
-      <c r="H78" t="s">
+      <c r="H79" t="s">
         <v>272</v>
       </c>
-      <c r="J78" t="s">
+      <c r="J79" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+    <row r="80" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>42</v>
       </c>
-      <c r="B79" t="s">
-        <v>168</v>
-      </c>
-      <c r="C79" s="36">
+      <c r="B80" t="s">
+        <v>168</v>
+      </c>
+      <c r="C80" s="36">
         <v>0.96699999999999997</v>
-      </c>
-      <c r="F79" t="s">
-        <v>81</v>
-      </c>
-      <c r="H79" t="s">
-        <v>282</v>
-      </c>
-      <c r="J79" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>10</v>
-      </c>
-      <c r="B80" t="s">
-        <v>168</v>
-      </c>
-      <c r="C80" s="9">
-        <v>0.98199999999999998</v>
       </c>
       <c r="F80" t="s">
         <v>81</v>
       </c>
       <c r="H80" t="s">
+        <v>282</v>
+      </c>
+      <c r="J80" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>10</v>
+      </c>
+      <c r="B81" t="s">
+        <v>168</v>
+      </c>
+      <c r="C81" s="9">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="F81" t="s">
+        <v>81</v>
+      </c>
+      <c r="H81" t="s">
         <v>230</v>
       </c>
-      <c r="J80" t="s">
+      <c r="J81" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>9</v>
       </c>
-      <c r="B81" t="s">
-        <v>168</v>
-      </c>
-      <c r="C81" s="9">
+      <c r="B82" t="s">
+        <v>168</v>
+      </c>
+      <c r="C82" s="9">
         <v>0.98299999999999998</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F82" t="s">
         <v>82</v>
       </c>
-      <c r="H81" t="s">
+      <c r="H82" t="s">
         <v>231</v>
       </c>
-      <c r="J81" t="s">
+      <c r="J82" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>53</v>
-      </c>
-      <c r="B82" t="s">
-        <v>169</v>
-      </c>
-      <c r="C82" s="42">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F82" t="s">
-        <v>309</v>
-      </c>
-      <c r="H82" t="s">
-        <v>310</v>
-      </c>
-      <c r="J82" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B83" t="s">
         <v>169</v>
       </c>
       <c r="C83" s="42">
-        <v>0.13800000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F83" t="s">
+        <v>308</v>
+      </c>
+      <c r="H83" t="s">
         <v>309</v>
       </c>
-      <c r="H83" t="s">
-        <v>311</v>
-      </c>
       <c r="J83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B84" t="s">
-        <v>170</v>
-      </c>
-      <c r="C84" s="43">
-        <v>0.16300000000000001</v>
+        <v>169</v>
+      </c>
+      <c r="C84" s="42">
+        <v>0.13800000000000001</v>
       </c>
       <c r="F84" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H84" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J84" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B85" t="s">
         <v>170</v>
       </c>
-      <c r="C85" s="42">
-        <v>0.13700000000000001</v>
+      <c r="C85" s="43">
+        <v>0.16300000000000001</v>
       </c>
       <c r="F85" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H85" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J85" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B86" t="s">
         <v>170</v>
       </c>
-      <c r="C86" s="44">
-        <v>0.9</v>
+      <c r="C86" s="42">
+        <v>0.13700000000000001</v>
       </c>
       <c r="F86" t="s">
-        <v>81</v>
+        <v>308</v>
       </c>
       <c r="H86" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="J86" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="61" t="s">
-        <v>58</v>
+      <c r="A87" t="s">
+        <v>57</v>
       </c>
       <c r="B87" t="s">
         <v>170</v>
       </c>
-      <c r="C87" s="45">
-        <v>0.32700000000000001</v>
+      <c r="C87" s="44">
+        <v>0.9</v>
       </c>
       <c r="F87" t="s">
         <v>81</v>
       </c>
       <c r="H87" t="s">
-        <v>315</v>
-      </c>
-      <c r="J87" s="61" t="s">
-        <v>178</v>
+        <v>313</v>
+      </c>
+      <c r="J87" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>59</v>
+      <c r="A88" s="61" t="s">
+        <v>58</v>
       </c>
       <c r="B88" t="s">
         <v>170</v>
       </c>
-      <c r="C88" s="46">
-        <v>0.64300000000000002</v>
+      <c r="C88" s="45">
+        <v>0.32700000000000001</v>
       </c>
       <c r="F88" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H88" t="s">
-        <v>270</v>
-      </c>
-      <c r="J88" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
+        <v>314</v>
+      </c>
+      <c r="J88" s="61" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>380</v>
+        <v>59</v>
       </c>
       <c r="B89" t="s">
         <v>170</v>
       </c>
-      <c r="C89" s="5">
-        <v>0</v>
+      <c r="C89" s="46">
+        <v>0.64300000000000002</v>
       </c>
       <c r="F89" t="s">
         <v>80</v>
       </c>
-      <c r="G89" s="3" t="s">
-        <v>262</v>
-      </c>
       <c r="H89" t="s">
-        <v>316</v>
-      </c>
-      <c r="I89" t="s">
-        <v>344</v>
+        <v>270</v>
       </c>
       <c r="J89" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B90" t="s">
         <v>170</v>
@@ -4778,15 +4795,18 @@
         <v>262</v>
       </c>
       <c r="H90" t="s">
-        <v>317</v>
+        <v>315</v>
+      </c>
+      <c r="I90" t="s">
+        <v>343</v>
       </c>
       <c r="J90" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="91" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B91" t="s">
         <v>170</v>
@@ -4801,15 +4821,15 @@
         <v>262</v>
       </c>
       <c r="H91" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="J91" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B92" t="s">
         <v>170</v>
@@ -4824,15 +4844,15 @@
         <v>262</v>
       </c>
       <c r="H92" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="J92" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B93" t="s">
         <v>170</v>
@@ -4847,15 +4867,15 @@
         <v>262</v>
       </c>
       <c r="H93" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="J93" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B94" t="s">
         <v>170</v>
@@ -4870,15 +4890,15 @@
         <v>262</v>
       </c>
       <c r="H94" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="J94" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B95" t="s">
         <v>170</v>
@@ -4893,15 +4913,15 @@
         <v>262</v>
       </c>
       <c r="H95" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="J95" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B96" t="s">
         <v>170</v>
@@ -4916,179 +4936,179 @@
         <v>262</v>
       </c>
       <c r="H96" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J96" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>60</v>
+        <v>386</v>
       </c>
       <c r="B97" t="s">
         <v>170</v>
       </c>
-      <c r="C97" s="9">
-        <v>0.98199999999999998</v>
+      <c r="C97" s="5">
+        <v>0</v>
       </c>
       <c r="F97" t="s">
-        <v>273</v>
+        <v>80</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>262</v>
       </c>
       <c r="H97" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="J97" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B98" t="s">
         <v>170</v>
       </c>
-      <c r="C98" s="47">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="D98" s="3" t="s">
-        <v>462</v>
+      <c r="C98" s="9">
+        <v>0.98199999999999998</v>
       </c>
       <c r="F98" t="s">
-        <v>82</v>
-      </c>
-      <c r="G98" t="s">
-        <v>345</v>
+        <v>273</v>
       </c>
       <c r="H98" t="s">
-        <v>274</v>
-      </c>
-      <c r="I98" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="J98" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" ht="102" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="63" t="s">
-        <v>62</v>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>61</v>
       </c>
       <c r="B99" t="s">
         <v>170</v>
       </c>
-      <c r="C99" s="48">
-        <v>0.38700000000000001</v>
+      <c r="C99" s="47">
+        <v>0.28000000000000003</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="F99" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G99" t="s">
-        <v>464</v>
+        <v>344</v>
       </c>
       <c r="H99" t="s">
-        <v>325</v>
+        <v>274</v>
       </c>
       <c r="I99" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J99" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
-        <v>63</v>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="102" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="63" t="s">
+        <v>62</v>
       </c>
       <c r="B100" t="s">
         <v>170</v>
       </c>
-      <c r="C100" s="49">
-        <v>0.73</v>
+      <c r="C100" s="48">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>459</v>
       </c>
       <c r="F100" t="s">
-        <v>309</v>
+        <v>80</v>
+      </c>
+      <c r="G100" t="s">
+        <v>458</v>
       </c>
       <c r="H100" t="s">
-        <v>326</v>
+        <v>324</v>
+      </c>
+      <c r="I100" t="s">
+        <v>327</v>
       </c>
       <c r="J100" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="63" t="s">
-        <v>64</v>
+      <c r="A101" t="s">
+        <v>63</v>
       </c>
       <c r="B101" t="s">
         <v>170</v>
       </c>
-      <c r="C101" s="50">
-        <v>0.158</v>
+      <c r="C101" s="49">
+        <v>0.73</v>
       </c>
       <c r="F101" t="s">
-        <v>80</v>
-      </c>
-      <c r="G101" t="s">
-        <v>329</v>
+        <v>308</v>
       </c>
       <c r="H101" t="s">
-        <v>283</v>
+        <v>325</v>
       </c>
       <c r="J101" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>65</v>
+      <c r="A102" s="63" t="s">
+        <v>64</v>
       </c>
       <c r="B102" t="s">
         <v>170</v>
       </c>
-      <c r="C102" s="51">
-        <v>0.21199999999999999</v>
+      <c r="C102" s="50">
+        <v>0.158</v>
       </c>
       <c r="F102" t="s">
         <v>80</v>
       </c>
+      <c r="G102" t="s">
+        <v>328</v>
+      </c>
       <c r="H102" t="s">
-        <v>330</v>
+        <v>283</v>
       </c>
       <c r="J102" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>388</v>
+        <v>65</v>
       </c>
       <c r="B103" t="s">
         <v>170</v>
       </c>
-      <c r="C103" s="5">
-        <v>0</v>
+      <c r="C103" s="51">
+        <v>0.21199999999999999</v>
       </c>
       <c r="F103" t="s">
         <v>80</v>
       </c>
-      <c r="G103" t="s">
-        <v>343</v>
-      </c>
       <c r="H103" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="J103" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B104" t="s">
         <v>170</v>
@@ -5099,114 +5119,111 @@
       <c r="F104" t="s">
         <v>80</v>
       </c>
+      <c r="G104" t="s">
+        <v>342</v>
+      </c>
       <c r="H104" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="J104" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>66</v>
+        <v>388</v>
       </c>
       <c r="B105" t="s">
         <v>170</v>
       </c>
-      <c r="C105" s="52">
-        <v>0.62</v>
+      <c r="C105" s="5">
+        <v>0</v>
       </c>
       <c r="F105" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H105" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="J105" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B106" t="s">
         <v>170</v>
       </c>
-      <c r="C106" s="53">
-        <v>0.442</v>
+      <c r="C106" s="52">
+        <v>0.62</v>
       </c>
       <c r="F106" t="s">
-        <v>82</v>
-      </c>
-      <c r="G106" t="s">
-        <v>345</v>
+        <v>81</v>
       </c>
       <c r="H106" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="J106" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" ht="68" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="63" t="s">
-        <v>68</v>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>67</v>
       </c>
       <c r="B107" t="s">
         <v>170</v>
       </c>
-      <c r="C107" s="54">
-        <v>0.125</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>411</v>
+      <c r="C107" s="53">
+        <v>0.442</v>
       </c>
       <c r="F107" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G107" t="s">
-        <v>301</v>
+        <v>344</v>
       </c>
       <c r="H107" t="s">
-        <v>335</v>
-      </c>
-      <c r="I107" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="J107" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>390</v>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="68" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="63" t="s">
+        <v>68</v>
       </c>
       <c r="B108" t="s">
         <v>170</v>
       </c>
-      <c r="C108" s="5">
-        <v>0</v>
+      <c r="C108" s="54">
+        <v>0.125</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="F108" t="s">
         <v>80</v>
       </c>
-      <c r="G108" s="3" t="s">
-        <v>262</v>
+      <c r="G108" t="s">
+        <v>300</v>
       </c>
       <c r="H108" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="I108" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="J108" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B109" t="s">
         <v>170</v>
@@ -5217,19 +5234,22 @@
       <c r="F109" t="s">
         <v>80</v>
       </c>
-      <c r="G109" t="s">
+      <c r="G109" s="3" t="s">
         <v>262</v>
       </c>
       <c r="H109" t="s">
-        <v>349</v>
+        <v>347</v>
+      </c>
+      <c r="I109" t="s">
+        <v>346</v>
       </c>
       <c r="J109" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B110" t="s">
         <v>170</v>
@@ -5244,15 +5264,15 @@
         <v>262</v>
       </c>
       <c r="H110" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="J110" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B111" t="s">
         <v>170</v>
@@ -5267,15 +5287,15 @@
         <v>262</v>
       </c>
       <c r="H111" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="J111" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B112" t="s">
         <v>170</v>
@@ -5290,15 +5310,15 @@
         <v>262</v>
       </c>
       <c r="H112" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="J112" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B113" t="s">
         <v>170</v>
@@ -5313,15 +5333,15 @@
         <v>262</v>
       </c>
       <c r="H113" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="J113" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B114" t="s">
         <v>170</v>
@@ -5336,84 +5356,87 @@
         <v>262</v>
       </c>
       <c r="H114" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="J114" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>69</v>
+        <v>395</v>
       </c>
       <c r="B115" t="s">
         <v>170</v>
       </c>
-      <c r="C115" s="55">
-        <v>0.32200000000000001</v>
+      <c r="C115" s="5">
+        <v>0</v>
       </c>
       <c r="F115" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="G115" t="s">
+        <v>262</v>
       </c>
       <c r="H115" t="s">
-        <v>282</v>
+        <v>353</v>
       </c>
       <c r="J115" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" ht="68" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="63" t="s">
-        <v>70</v>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>69</v>
       </c>
       <c r="B116" t="s">
         <v>170</v>
       </c>
-      <c r="C116" s="42">
-        <v>0.13800000000000001</v>
-      </c>
-      <c r="D116" s="3" t="s">
-        <v>411</v>
+      <c r="C116" s="55">
+        <v>0.32200000000000001</v>
       </c>
       <c r="F116" t="s">
-        <v>80</v>
-      </c>
-      <c r="G116" t="s">
-        <v>301</v>
+        <v>81</v>
       </c>
       <c r="H116" t="s">
-        <v>336</v>
-      </c>
-      <c r="I116" t="s">
-        <v>329</v>
+        <v>282</v>
       </c>
       <c r="J116" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>71</v>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" ht="68" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="63" t="s">
+        <v>70</v>
       </c>
       <c r="B117" t="s">
         <v>170</v>
       </c>
-      <c r="C117" s="56">
-        <v>0.77300000000000002</v>
+      <c r="C117" s="42">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="F117" t="s">
-        <v>309</v>
+        <v>80</v>
+      </c>
+      <c r="G117" t="s">
+        <v>300</v>
       </c>
       <c r="H117" t="s">
-        <v>337</v>
+        <v>335</v>
+      </c>
+      <c r="I117" t="s">
+        <v>328</v>
       </c>
       <c r="J117" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B118" t="s">
         <v>170</v>
@@ -5422,110 +5445,107 @@
         <v>0.77300000000000002</v>
       </c>
       <c r="F118" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H118" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="J118" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B119" t="s">
         <v>170</v>
       </c>
-      <c r="C119" s="25">
-        <v>0.78700000000000003</v>
+      <c r="C119" s="56">
+        <v>0.77300000000000002</v>
       </c>
       <c r="F119" t="s">
-        <v>81</v>
+        <v>308</v>
       </c>
       <c r="H119" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="J119" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B120" t="s">
         <v>170</v>
       </c>
-      <c r="C120" s="57">
-        <v>0.13200000000000001</v>
+      <c r="C120" s="25">
+        <v>0.78700000000000003</v>
       </c>
       <c r="F120" t="s">
-        <v>80</v>
-      </c>
-      <c r="G120" t="s">
-        <v>355</v>
+        <v>81</v>
       </c>
       <c r="H120" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="J120" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B121" t="s">
         <v>170</v>
       </c>
-      <c r="C121" s="58">
-        <v>0.93300000000000005</v>
+      <c r="C121" s="57">
+        <v>0.13200000000000001</v>
       </c>
       <c r="F121" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="G121" t="s">
+        <v>354</v>
       </c>
       <c r="H121" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="J121" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B122" t="s">
         <v>170</v>
       </c>
-      <c r="C122" s="6">
-        <v>1.2999999999999999E-2</v>
+      <c r="C122" s="58">
+        <v>0.93300000000000005</v>
       </c>
       <c r="F122" t="s">
-        <v>80</v>
-      </c>
-      <c r="G122" t="s">
-        <v>262</v>
+        <v>81</v>
       </c>
       <c r="H122" t="s">
-        <v>475</v>
+        <v>340</v>
       </c>
       <c r="J122" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B123" t="s">
         <v>170</v>
       </c>
-      <c r="C123" s="59">
-        <v>0.307</v>
+      <c r="C123" s="6">
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="F123" t="s">
         <v>80</v>
@@ -5534,21 +5554,21 @@
         <v>262</v>
       </c>
       <c r="H123" t="s">
-        <v>342</v>
+        <v>469</v>
       </c>
       <c r="J123" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B124" t="s">
         <v>170</v>
       </c>
-      <c r="C124" s="5">
-        <v>0</v>
+      <c r="C124" s="59">
+        <v>0.307</v>
       </c>
       <c r="F124" t="s">
         <v>80</v>
@@ -5557,29 +5577,38 @@
         <v>262</v>
       </c>
       <c r="H124" t="s">
-        <v>412</v>
+        <v>341</v>
       </c>
       <c r="J124" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>78</v>
+      </c>
+      <c r="B125" t="s">
+        <v>170</v>
+      </c>
+      <c r="C125" s="5">
+        <v>0</v>
+      </c>
+      <c r="F125" t="s">
+        <v>80</v>
+      </c>
+      <c r="G125" t="s">
+        <v>262</v>
+      </c>
+      <c r="H125" t="s">
+        <v>411</v>
+      </c>
+      <c r="J125" t="s">
         <v>215</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
-        <v>308</v>
-      </c>
-      <c r="B125" t="s">
-        <v>168</v>
-      </c>
-      <c r="F125" t="s">
-        <v>81</v>
-      </c>
-      <c r="H125" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>404</v>
+        <v>307</v>
       </c>
       <c r="B126" t="s">
         <v>168</v>
@@ -5588,12 +5617,12 @@
         <v>81</v>
       </c>
       <c r="H126" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A127" s="64" t="s">
-        <v>356</v>
+        <v>471</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>403</v>
       </c>
       <c r="B127" t="s">
         <v>168</v>
@@ -5602,74 +5631,74 @@
         <v>81</v>
       </c>
       <c r="H127" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A128" s="64" t="s">
+        <v>355</v>
+      </c>
+      <c r="B128" t="s">
+        <v>168</v>
+      </c>
+      <c r="F128" t="s">
+        <v>81</v>
+      </c>
+      <c r="H128" s="67" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="64" t="s">
+        <v>356</v>
+      </c>
+      <c r="B129" t="s">
+        <v>168</v>
+      </c>
+      <c r="F129" t="s">
+        <v>80</v>
+      </c>
+      <c r="G129" t="s">
+        <v>300</v>
+      </c>
+      <c r="H129" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>357</v>
       </c>
-      <c r="B128" t="s">
-        <v>168</v>
-      </c>
-      <c r="F128" t="s">
-        <v>80</v>
-      </c>
-      <c r="G128" t="s">
-        <v>301</v>
-      </c>
-      <c r="H128" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>358</v>
-      </c>
-      <c r="B129" t="s">
-        <v>168</v>
-      </c>
-      <c r="F129" t="s">
+      <c r="B130" t="s">
+        <v>168</v>
+      </c>
+      <c r="F130" t="s">
         <v>81</v>
       </c>
-      <c r="H129" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>474</v>
-      </c>
-      <c r="B130" t="s">
-        <v>168</v>
-      </c>
-      <c r="F130" t="s">
-        <v>80</v>
-      </c>
-      <c r="G130" t="s">
-        <v>301</v>
-      </c>
-      <c r="H130" t="s">
+      <c r="H130" s="67" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="B131" t="s">
         <v>168</v>
       </c>
       <c r="F131" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="G131" t="s">
+        <v>300</v>
       </c>
       <c r="H131" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>405</v>
+        <v>451</v>
       </c>
       <c r="B132" t="s">
         <v>168</v>
@@ -5678,77 +5707,74 @@
         <v>81</v>
       </c>
       <c r="H132" t="s">
-        <v>467</v>
+        <v>452</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>466</v>
+        <v>404</v>
       </c>
       <c r="B133" t="s">
         <v>168</v>
       </c>
       <c r="F133" t="s">
-        <v>80</v>
-      </c>
-      <c r="G133" t="s">
-        <v>301</v>
+        <v>81</v>
       </c>
       <c r="H133" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>359</v>
+        <v>460</v>
       </c>
       <c r="B134" t="s">
         <v>168</v>
       </c>
       <c r="F134" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="G134" t="s">
+        <v>300</v>
       </c>
       <c r="H134" t="s">
-        <v>422</v>
+        <v>462</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>406</v>
+        <v>358</v>
       </c>
       <c r="B135" t="s">
         <v>168</v>
       </c>
       <c r="F135" t="s">
-        <v>309</v>
+        <v>81</v>
       </c>
       <c r="H135" t="s">
-        <v>281</v>
-      </c>
-      <c r="J135" t="s">
-        <v>147</v>
+        <v>421</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>37</v>
+        <v>405</v>
       </c>
       <c r="B136" t="s">
         <v>168</v>
       </c>
       <c r="F136" t="s">
-        <v>81</v>
+        <v>308</v>
       </c>
       <c r="H136" t="s">
-        <v>408</v>
+        <v>281</v>
       </c>
       <c r="J136" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>407</v>
+        <v>37</v>
       </c>
       <c r="B137" t="s">
         <v>168</v>
@@ -5757,83 +5783,80 @@
         <v>81</v>
       </c>
       <c r="H137" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="J137" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A138" s="63" t="s">
-        <v>459</v>
+      <c r="A138" t="s">
+        <v>406</v>
       </c>
       <c r="B138" t="s">
+        <v>168</v>
+      </c>
+      <c r="F138" t="s">
+        <v>81</v>
+      </c>
+      <c r="H138" t="s">
+        <v>408</v>
+      </c>
+      <c r="J138" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A139" s="63" t="s">
+        <v>453</v>
+      </c>
+      <c r="B139" t="s">
         <v>170</v>
       </c>
-      <c r="F138" t="s">
-        <v>80</v>
-      </c>
-      <c r="G138" t="s">
+      <c r="F139" t="s">
+        <v>80</v>
+      </c>
+      <c r="G139" t="s">
         <v>262</v>
       </c>
-      <c r="H138" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
-        <v>415</v>
-      </c>
-      <c r="B139" t="s">
-        <v>168</v>
-      </c>
-      <c r="F139" t="s">
-        <v>80</v>
-      </c>
-      <c r="G139" t="s">
-        <v>301</v>
-      </c>
       <c r="H139" t="s">
-        <v>423</v>
+        <v>454</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B140" t="s">
         <v>168</v>
       </c>
       <c r="F140" t="s">
+        <v>80</v>
+      </c>
+      <c r="G140" t="s">
+        <v>300</v>
+      </c>
+      <c r="H140" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>415</v>
+      </c>
+      <c r="B141" t="s">
+        <v>168</v>
+      </c>
+      <c r="F141" t="s">
         <v>81</v>
       </c>
-      <c r="H140" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A141" s="60" t="s">
-        <v>417</v>
-      </c>
-      <c r="B141" s="60" t="s">
-        <v>168</v>
-      </c>
-      <c r="C141" s="62"/>
-      <c r="D141" s="60"/>
-      <c r="E141" s="60"/>
-      <c r="F141" s="60" t="s">
-        <v>80</v>
-      </c>
-      <c r="G141" s="60" t="s">
-        <v>301</v>
-      </c>
-      <c r="H141" s="60" t="s">
-        <v>425</v>
+      <c r="H141" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" s="60" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B142" s="60" t="s">
         <v>168</v>
@@ -5842,16 +5865,18 @@
       <c r="D142" s="60"/>
       <c r="E142" s="60"/>
       <c r="F142" s="60" t="s">
-        <v>81</v>
-      </c>
-      <c r="G142" s="60"/>
+        <v>80</v>
+      </c>
+      <c r="G142" s="60" t="s">
+        <v>300</v>
+      </c>
       <c r="H142" s="60" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" s="60" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B143" s="60" t="s">
         <v>168</v>
@@ -5860,18 +5885,16 @@
       <c r="D143" s="60"/>
       <c r="E143" s="60"/>
       <c r="F143" s="60" t="s">
-        <v>80</v>
-      </c>
-      <c r="G143" s="60" t="s">
-        <v>301</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="G143" s="60"/>
       <c r="H143" s="60" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" s="60" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B144" s="60" t="s">
         <v>168</v>
@@ -5880,39 +5903,76 @@
       <c r="D144" s="60"/>
       <c r="E144" s="60"/>
       <c r="F144" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="G144" s="60" t="s">
+        <v>300</v>
+      </c>
+      <c r="H144" s="60" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A145" s="60" t="s">
+        <v>419</v>
+      </c>
+      <c r="B145" s="60" t="s">
+        <v>168</v>
+      </c>
+      <c r="C145" s="62"/>
+      <c r="D145" s="60"/>
+      <c r="E145" s="60"/>
+      <c r="F145" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="G144" s="60"/>
-      <c r="H144" s="60" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
-        <v>469</v>
-      </c>
-      <c r="B145" s="60" t="s">
-        <v>168</v>
-      </c>
-      <c r="F145" s="60" t="s">
-        <v>309</v>
-      </c>
+      <c r="G145" s="60"/>
       <c r="H145" s="60" t="s">
-        <v>470</v>
+        <v>427</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A146" s="60" t="s">
+        <v>472</v>
+      </c>
+      <c r="B146" s="60" t="s">
+        <v>168</v>
+      </c>
+      <c r="F146" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="G146" t="s">
+        <v>262</v>
+      </c>
+      <c r="H146" s="60" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>463</v>
+      </c>
+      <c r="B147" s="60" t="s">
+        <v>168</v>
+      </c>
+      <c r="F147" s="60" t="s">
+        <v>308</v>
+      </c>
+      <c r="H147" s="60" t="s">
+        <v>464</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J124" xr:uid="{05D32D06-7DAE-3944-9C50-40C3579C6515}">
+  <autoFilter ref="A1:J125" xr:uid="{05D32D06-7DAE-3944-9C50-40C3579C6515}">
     <filterColumn colId="1">
       <filters>
         <filter val="PRE"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J81">
-      <sortCondition sortBy="cellColor" ref="A1:A124" dxfId="0"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J82">
+      <sortCondition sortBy="cellColor" ref="A1:A125" dxfId="0"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="C145:C1048576 C134:C140 C125:C131">
+  <conditionalFormatting sqref="C146:C1048576 C135:C141 C126:C132">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -5922,7 +5982,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C132:C133">
+  <conditionalFormatting sqref="C133:C134">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
improved calculater UI and function (better captions, explanation of logit fn, rounding, and etc
</commit_message>
<xml_diff>
--- a/data/Metadata.xlsx
+++ b/data/Metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yifu/Documents/github-repo/iibr-pmrt-calculator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2040FCB-4D0B-F54D-AEDF-A0651B803FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B193AD-F463-9545-9C55-874921261514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3920" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{2D76DBCA-B48D-704D-8521-B15612E5208C}"/>
   </bookViews>
@@ -1719,15 +1719,6 @@
     <t>Presence of metastatic carcinoma on axillary lymph node biopsy</t>
   </si>
   <si>
-    <t>Histology subtype is DCIS</t>
-  </si>
-  <si>
-    <t>Histology subtype is IDC</t>
-  </si>
-  <si>
-    <t>Presence of pre-operative suspicious/palpable lymph node or lymphadenopathy</t>
-  </si>
-  <si>
     <t>Maximum dimension/size of pre-operative tumor</t>
   </si>
   <si>
@@ -1737,16 +1728,25 @@
     <t>Initial diagnostic imaging modality is ultrasound</t>
   </si>
   <si>
-    <t>Pre-operative biopsy method</t>
-  </si>
-  <si>
-    <t>Surgical indication – primary treatment</t>
-  </si>
-  <si>
     <t>Initial diagnostic imaging modality is mammography</t>
   </si>
   <si>
-    <t>Surgical indication – recurrent cancer</t>
+    <t>Presence of pre-operative suspicious lymph node, palpable lymph node, or lymphadenopathy</t>
+  </si>
+  <si>
+    <t>Histology subtype is Ductal Carcinoma In Situ (DCIS)</t>
+  </si>
+  <si>
+    <t>Histology subtype is Invasive Ductal Carcinoma (IDC)</t>
+  </si>
+  <si>
+    <t>Pre-operative biopsy method used</t>
+  </si>
+  <si>
+    <t>Surgical indication is primary treatment</t>
+  </si>
+  <si>
+    <t>Surgical indication is recurrent cancer</t>
   </si>
 </sst>
 </file>
@@ -2289,7 +2289,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2577,7 +2577,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2671,9 +2671,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="113" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H43" sqref="A1:J147 A123:J147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3441,7 +3441,7 @@
         <v>262</v>
       </c>
       <c r="H31" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="I31" t="s">
         <v>234</v>
@@ -3467,7 +3467,7 @@
         <v>262</v>
       </c>
       <c r="H32" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="J32" t="s">
         <v>112</v>
@@ -3513,7 +3513,7 @@
         <v>262</v>
       </c>
       <c r="H34" s="66" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="I34" t="s">
         <v>271</v>
@@ -3562,7 +3562,7 @@
         <v>262</v>
       </c>
       <c r="H36" s="66" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
       <c r="J36" t="s">
         <v>139</v>
@@ -3657,7 +3657,7 @@
         <v>262</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="I40" s="3" t="s">
         <v>291</v>
@@ -3967,7 +3967,7 @@
         <v>269</v>
       </c>
       <c r="H53" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="J53" t="s">
         <v>174</v>
@@ -5645,7 +5645,7 @@
         <v>81</v>
       </c>
       <c r="H128" s="67" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="129" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -5662,7 +5662,7 @@
         <v>300</v>
       </c>
       <c r="H129" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
     </row>
     <row r="130" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -5676,7 +5676,7 @@
         <v>81</v>
       </c>
       <c r="H130" s="67" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added units to sliding bar
</commit_message>
<xml_diff>
--- a/data/Metadata.xlsx
+++ b/data/Metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yifu/Documents/github-repo/iibr-pmrt-calculator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B193AD-F463-9545-9C55-874921261514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8055C0BE-83D3-D549-842A-0C73F577D235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3920" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{2D76DBCA-B48D-704D-8521-B15612E5208C}"/>
   </bookViews>
@@ -1719,12 +1719,6 @@
     <t>Presence of metastatic carcinoma on axillary lymph node biopsy</t>
   </si>
   <si>
-    <t>Maximum dimension/size of pre-operative tumor</t>
-  </si>
-  <si>
-    <t>Maximum size of pre-operative suspicious lymph node</t>
-  </si>
-  <si>
     <t>Initial diagnostic imaging modality is ultrasound</t>
   </si>
   <si>
@@ -1747,6 +1741,12 @@
   </si>
   <si>
     <t>Surgical indication is recurrent cancer</t>
+  </si>
+  <si>
+    <t>Maximum size of pre-operative suspicious lymph node (measured in mm)</t>
+  </si>
+  <si>
+    <t>Maximum dimension/size of pre-operative tumor (measured in mm)</t>
   </si>
 </sst>
 </file>
@@ -2672,8 +2672,8 @@
   <dimension ref="A1:J147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H43" sqref="A1:J147 A123:J147"/>
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H131" sqref="H131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3441,7 +3441,7 @@
         <v>262</v>
       </c>
       <c r="H31" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="I31" t="s">
         <v>234</v>
@@ -3467,7 +3467,7 @@
         <v>262</v>
       </c>
       <c r="H32" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="J32" t="s">
         <v>112</v>
@@ -3513,7 +3513,7 @@
         <v>262</v>
       </c>
       <c r="H34" s="66" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="I34" t="s">
         <v>271</v>
@@ -3562,7 +3562,7 @@
         <v>262</v>
       </c>
       <c r="H36" s="66" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="J36" t="s">
         <v>139</v>
@@ -3657,7 +3657,7 @@
         <v>262</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="I40" s="3" t="s">
         <v>291</v>
@@ -3729,7 +3729,7 @@
         <v>262</v>
       </c>
       <c r="H43" s="67" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="J43" t="s">
         <v>159</v>
@@ -3967,7 +3967,7 @@
         <v>269</v>
       </c>
       <c r="H53" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="J53" t="s">
         <v>174</v>
@@ -5645,7 +5645,7 @@
         <v>81</v>
       </c>
       <c r="H128" s="67" t="s">
-        <v>476</v>
+        <v>483</v>
       </c>
     </row>
     <row r="129" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -5662,7 +5662,7 @@
         <v>300</v>
       </c>
       <c r="H129" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="130" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -5676,7 +5676,7 @@
         <v>81</v>
       </c>
       <c r="H130" s="67" t="s">
-        <v>475</v>
+        <v>484</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
small syntax improvement in writing
</commit_message>
<xml_diff>
--- a/data/Metadata.xlsx
+++ b/data/Metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yifu/Documents/github-repo/iibr-pmrt-calculator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8055C0BE-83D3-D549-842A-0C73F577D235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A21C3C9-B39D-864B-ACBA-4B32BDA35925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3920" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{2D76DBCA-B48D-704D-8521-B15612E5208C}"/>
   </bookViews>
@@ -1743,10 +1743,10 @@
     <t>Surgical indication is recurrent cancer</t>
   </si>
   <si>
-    <t>Maximum size of pre-operative suspicious lymph node (measured in mm)</t>
-  </si>
-  <si>
-    <t>Maximum dimension/size of pre-operative tumor (measured in mm)</t>
+    <t>Maximum size of pre-operative suspicious lymph node across modalities (measured in mm; slide to 0 if there is no pre-operative suspicious LN)</t>
+  </si>
+  <si>
+    <t>Maximum dimension/size of pre-operative tumor across modalities (measured in mm; modality could be mammography, PET, or ultrasound)</t>
   </si>
 </sst>
 </file>
@@ -2671,8 +2671,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="113" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H131" sqref="H131"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
improve calculator according to feedback
</commit_message>
<xml_diff>
--- a/data/Metadata.xlsx
+++ b/data/Metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yifu/Documents/github-repo/iibr-pmrt-calculator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A21C3C9-B39D-864B-ACBA-4B32BDA35925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C040D1-7D9A-424B-AB4F-48F8DEAA22E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3920" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{2D76DBCA-B48D-704D-8521-B15612E5208C}"/>
   </bookViews>
@@ -267,7 +267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="486">
   <si>
     <t>Field</t>
   </si>
@@ -1082,9 +1082,6 @@
     <t>Pre-operative biopsy date</t>
   </si>
   <si>
-    <t>1, CNB | 2, surgical biopsy | 3, FNA | 4, other</t>
-  </si>
-  <si>
     <t>Tumor location (clock orientation)</t>
   </si>
   <si>
@@ -1142,9 +1139,6 @@
   </si>
   <si>
     <t xml:space="preserve">Imaging and biopsy concordance </t>
-  </si>
-  <si>
-    <t>Axillary lymph node core biopsy or FNA</t>
   </si>
   <si>
     <t>if val == 2:
@@ -1725,9 +1719,6 @@
     <t>Initial diagnostic imaging modality is mammography</t>
   </si>
   <si>
-    <t>Presence of pre-operative suspicious lymph node, palpable lymph node, or lymphadenopathy</t>
-  </si>
-  <si>
     <t>Histology subtype is Ductal Carcinoma In Situ (DCIS)</t>
   </si>
   <si>
@@ -1743,10 +1734,22 @@
     <t>Surgical indication is recurrent cancer</t>
   </si>
   <si>
-    <t>Maximum size of pre-operative suspicious lymph node across modalities (measured in mm; slide to 0 if there is no pre-operative suspicious LN)</t>
-  </si>
-  <si>
-    <t>Maximum dimension/size of pre-operative tumor across modalities (measured in mm; modality could be mammography, PET, or ultrasound)</t>
+    <t>Presence of pre-operative palpable lymph node</t>
+  </si>
+  <si>
+    <t>Axillary lymph node core biopsy performed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, positive | 2, negative </t>
+  </si>
+  <si>
+    <t>Maximum size of pre-operative suspicious lymph node on any imaging modality (measured in mm; select 0 if there is no pre-operative suspecious LN)</t>
+  </si>
+  <si>
+    <t>Maximum dimension/size of pre-operative tumor on any imaging modality (measured in mm)</t>
+  </si>
+  <si>
+    <t>1, CNB | 2, surgical biopsy | 3, FNA</t>
   </si>
 </sst>
 </file>
@@ -2671,9 +2674,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="113" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H131" sqref="H131"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2696,7 +2699,7 @@
         <v>167</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>236</v>
@@ -2714,10 +2717,10 @@
         <v>84</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -2746,7 +2749,7 @@
         <v>217</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F3" t="s">
         <v>80</v>
@@ -2795,19 +2798,19 @@
         <v>6.2E-2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F5" t="s">
         <v>82</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>412</v>
+        <v>277</v>
       </c>
       <c r="H5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J5" t="s">
         <v>150</v>
@@ -2824,19 +2827,19 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F6" t="s">
         <v>82</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J6" t="s">
         <v>144</v>
@@ -2853,19 +2856,19 @@
         <v>0.153</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F7" t="s">
         <v>82</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="H7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J7" t="s">
         <v>151</v>
@@ -2882,19 +2885,19 @@
         <v>0.155</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F8" t="s">
         <v>82</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>412</v>
+        <v>482</v>
       </c>
       <c r="H8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J8" t="s">
         <v>152</v>
@@ -2917,10 +2920,10 @@
         <v>80</v>
       </c>
       <c r="G9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J9" t="s">
         <v>149</v>
@@ -3012,7 +3015,7 @@
         <v>0.66200000000000003</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E13" t="s">
         <v>235</v>
@@ -3021,10 +3024,10 @@
         <v>82</v>
       </c>
       <c r="G13" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H13" s="66" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="J13" t="s">
         <v>155</v>
@@ -3064,7 +3067,7 @@
         <v>0.98499999999999999</v>
       </c>
       <c r="E15" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F15" t="s">
         <v>81</v>
@@ -3110,7 +3113,7 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H17" t="s">
         <v>218</v>
@@ -3141,7 +3144,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B19" t="s">
         <v>168</v>
@@ -3156,7 +3159,7 @@
         <v>262</v>
       </c>
       <c r="H19" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="I19" t="s">
         <v>223</v>
@@ -3167,7 +3170,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B20" t="s">
         <v>168</v>
@@ -3182,7 +3185,7 @@
         <v>262</v>
       </c>
       <c r="H20" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="J20" t="s">
         <v>93</v>
@@ -3190,7 +3193,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B21" t="s">
         <v>168</v>
@@ -3205,7 +3208,7 @@
         <v>262</v>
       </c>
       <c r="H21" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J21" t="s">
         <v>94</v>
@@ -3213,7 +3216,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B22" t="s">
         <v>168</v>
@@ -3228,7 +3231,7 @@
         <v>262</v>
       </c>
       <c r="H22" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="J22" t="s">
         <v>95</v>
@@ -3236,7 +3239,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B23" t="s">
         <v>168</v>
@@ -3251,7 +3254,7 @@
         <v>262</v>
       </c>
       <c r="H23" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="J23" t="s">
         <v>96</v>
@@ -3259,7 +3262,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B24" t="s">
         <v>168</v>
@@ -3274,7 +3277,7 @@
         <v>262</v>
       </c>
       <c r="H24" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="J24" t="s">
         <v>97</v>
@@ -3282,7 +3285,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B25" t="s">
         <v>168</v>
@@ -3297,7 +3300,7 @@
         <v>262</v>
       </c>
       <c r="H25" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="J25" t="s">
         <v>98</v>
@@ -3305,7 +3308,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B26" t="s">
         <v>168</v>
@@ -3320,7 +3323,7 @@
         <v>262</v>
       </c>
       <c r="H26" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="I26" t="s">
         <v>224</v>
@@ -3331,7 +3334,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B27" t="s">
         <v>168</v>
@@ -3346,7 +3349,7 @@
         <v>262</v>
       </c>
       <c r="H27" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="J27" t="s">
         <v>100</v>
@@ -3354,7 +3357,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B28" t="s">
         <v>168</v>
@@ -3369,7 +3372,7 @@
         <v>262</v>
       </c>
       <c r="H28" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="J28" t="s">
         <v>101</v>
@@ -3377,7 +3380,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="64" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B29" t="s">
         <v>168</v>
@@ -3392,7 +3395,7 @@
         <v>262</v>
       </c>
       <c r="H29" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="J29" t="s">
         <v>102</v>
@@ -3400,7 +3403,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B30" t="s">
         <v>168</v>
@@ -3418,7 +3421,7 @@
         <v>262</v>
       </c>
       <c r="H30" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="J30" t="s">
         <v>103</v>
@@ -3426,7 +3429,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B31" t="s">
         <v>168</v>
@@ -3441,7 +3444,7 @@
         <v>262</v>
       </c>
       <c r="H31" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="I31" t="s">
         <v>234</v>
@@ -3452,7 +3455,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B32" t="s">
         <v>168</v>
@@ -3467,7 +3470,7 @@
         <v>262</v>
       </c>
       <c r="H32" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="J32" t="s">
         <v>112</v>
@@ -3475,7 +3478,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B33" t="s">
         <v>168</v>
@@ -3490,7 +3493,7 @@
         <v>262</v>
       </c>
       <c r="H33" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="J33" t="s">
         <v>113</v>
@@ -3498,7 +3501,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B34" t="s">
         <v>168</v>
@@ -3513,10 +3516,10 @@
         <v>262</v>
       </c>
       <c r="H34" s="66" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="I34" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J34" t="s">
         <v>137</v>
@@ -3524,7 +3527,7 @@
     </row>
     <row r="35" spans="1:10" ht="74" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B35" t="s">
         <v>168</v>
@@ -3539,7 +3542,7 @@
         <v>262</v>
       </c>
       <c r="H35" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="J35" t="s">
         <v>138</v>
@@ -3547,7 +3550,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B36" t="s">
         <v>168</v>
@@ -3562,7 +3565,7 @@
         <v>262</v>
       </c>
       <c r="H36" s="66" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="J36" t="s">
         <v>139</v>
@@ -3570,7 +3573,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B37" t="s">
         <v>168</v>
@@ -3585,7 +3588,7 @@
         <v>262</v>
       </c>
       <c r="H37" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="J37" t="s">
         <v>140</v>
@@ -3593,7 +3596,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B38" t="s">
         <v>168</v>
@@ -3608,7 +3611,7 @@
         <v>262</v>
       </c>
       <c r="H38" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="J38" t="s">
         <v>141</v>
@@ -3616,7 +3619,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B39" t="s">
         <v>168</v>
@@ -3631,7 +3634,7 @@
         <v>262</v>
       </c>
       <c r="H39" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="J39" t="s">
         <v>142</v>
@@ -3639,7 +3642,7 @@
     </row>
     <row r="40" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B40" t="s">
         <v>168</v>
@@ -3648,7 +3651,7 @@
         <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F40" t="s">
         <v>80</v>
@@ -3657,10 +3660,10 @@
         <v>262</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J40" t="s">
         <v>156</v>
@@ -3668,7 +3671,7 @@
     </row>
     <row r="41" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B41" t="s">
         <v>168</v>
@@ -3683,7 +3686,7 @@
         <v>262</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="J41" t="s">
         <v>157</v>
@@ -3691,7 +3694,7 @@
     </row>
     <row r="42" spans="1:10" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B42" t="s">
         <v>168</v>
@@ -3706,7 +3709,7 @@
         <v>262</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="J42" t="s">
         <v>158</v>
@@ -3714,7 +3717,7 @@
     </row>
     <row r="43" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="65" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B43" t="s">
         <v>168</v>
@@ -3729,7 +3732,7 @@
         <v>262</v>
       </c>
       <c r="H43" s="67" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="J43" t="s">
         <v>159</v>
@@ -3737,7 +3740,7 @@
     </row>
     <row r="44" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B44" t="s">
         <v>168</v>
@@ -3752,7 +3755,7 @@
         <v>262</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="J44" t="s">
         <v>160</v>
@@ -3760,7 +3763,7 @@
     </row>
     <row r="45" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="64" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B45" s="64" t="s">
         <v>170</v>
@@ -3778,10 +3781,10 @@
         <v>262</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="J45" t="s">
         <v>164</v>
@@ -3789,7 +3792,7 @@
     </row>
     <row r="46" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="64" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B46" s="64" t="s">
         <v>170</v>
@@ -3804,7 +3807,7 @@
         <v>262</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="J46" t="s">
         <v>165</v>
@@ -3812,7 +3815,7 @@
     </row>
     <row r="47" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="64" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B47" s="64" t="s">
         <v>170</v>
@@ -3827,7 +3830,7 @@
         <v>262</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="J47" t="s">
         <v>166</v>
@@ -3870,10 +3873,10 @@
         <v>80</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I49" s="3"/>
       <c r="J49" t="s">
@@ -3894,10 +3897,10 @@
         <v>80</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H50" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J50" t="s">
         <v>163</v>
@@ -3914,13 +3917,13 @@
         <v>1.2E-2</v>
       </c>
       <c r="E51" s="63" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F51" t="s">
         <v>79</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I51" s="3"/>
       <c r="J51" t="s">
@@ -3964,10 +3967,10 @@
         <v>80</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>269</v>
+        <v>485</v>
       </c>
       <c r="H53" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="J53" t="s">
         <v>174</v>
@@ -4007,7 +4010,7 @@
         <v>79</v>
       </c>
       <c r="H55" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J55" t="s">
         <v>114</v>
@@ -4044,7 +4047,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F57" t="s">
         <v>82</v>
@@ -4053,7 +4056,7 @@
         <v>247</v>
       </c>
       <c r="H57" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J57" t="s">
         <v>153</v>
@@ -4079,7 +4082,7 @@
         <v>262</v>
       </c>
       <c r="H58" t="s">
-        <v>289</v>
+        <v>481</v>
       </c>
       <c r="J58" t="s">
         <v>154</v>
@@ -4116,7 +4119,7 @@
         <v>0.24199999999999999</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E60" t="s">
         <v>235</v>
@@ -4148,7 +4151,7 @@
         <v>80</v>
       </c>
       <c r="H61" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J61" t="s">
         <v>135</v>
@@ -4258,7 +4261,7 @@
         <v>242</v>
       </c>
       <c r="F66" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H66" t="s">
         <v>241</v>
@@ -4347,7 +4350,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="60" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B70" t="s">
         <v>168</v>
@@ -4431,10 +4434,10 @@
         <v>82</v>
       </c>
       <c r="G73" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H73" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J73" t="s">
         <v>145</v>
@@ -4529,7 +4532,7 @@
         <v>80</v>
       </c>
       <c r="H77" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J77" t="s">
         <v>146</v>
@@ -4552,7 +4555,7 @@
         <v>81</v>
       </c>
       <c r="H78" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="J78" t="s">
         <v>130</v>
@@ -4569,10 +4572,10 @@
         <v>0.96299999999999997</v>
       </c>
       <c r="F79" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H79" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J79" t="s">
         <v>143</v>
@@ -4592,7 +4595,7 @@
         <v>81</v>
       </c>
       <c r="H80" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J80" t="s">
         <v>148</v>
@@ -4649,10 +4652,10 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="F83" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H83" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="J83" t="s">
         <v>171</v>
@@ -4669,10 +4672,10 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="F84" t="s">
+        <v>306</v>
+      </c>
+      <c r="H84" t="s">
         <v>308</v>
-      </c>
-      <c r="H84" t="s">
-        <v>310</v>
       </c>
       <c r="J84" t="s">
         <v>172</v>
@@ -4689,10 +4692,10 @@
         <v>0.16300000000000001</v>
       </c>
       <c r="F85" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H85" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="J85" t="s">
         <v>175</v>
@@ -4709,10 +4712,10 @@
         <v>0.13700000000000001</v>
       </c>
       <c r="F86" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H86" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J86" t="s">
         <v>176</v>
@@ -4732,7 +4735,7 @@
         <v>81</v>
       </c>
       <c r="H87" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J87" t="s">
         <v>177</v>
@@ -4752,7 +4755,7 @@
         <v>81</v>
       </c>
       <c r="H88" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="J88" s="61" t="s">
         <v>178</v>
@@ -4772,7 +4775,7 @@
         <v>80</v>
       </c>
       <c r="H89" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J89" t="s">
         <v>179</v>
@@ -4780,7 +4783,7 @@
     </row>
     <row r="90" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B90" t="s">
         <v>170</v>
@@ -4795,10 +4798,10 @@
         <v>262</v>
       </c>
       <c r="H90" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I90" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="J90" t="s">
         <v>180</v>
@@ -4806,7 +4809,7 @@
     </row>
     <row r="91" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B91" t="s">
         <v>170</v>
@@ -4821,7 +4824,7 @@
         <v>262</v>
       </c>
       <c r="H91" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="J91" t="s">
         <v>181</v>
@@ -4829,7 +4832,7 @@
     </row>
     <row r="92" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B92" t="s">
         <v>170</v>
@@ -4844,7 +4847,7 @@
         <v>262</v>
       </c>
       <c r="H92" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="J92" t="s">
         <v>182</v>
@@ -4852,7 +4855,7 @@
     </row>
     <row r="93" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B93" t="s">
         <v>170</v>
@@ -4867,7 +4870,7 @@
         <v>262</v>
       </c>
       <c r="H93" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="J93" t="s">
         <v>183</v>
@@ -4875,7 +4878,7 @@
     </row>
     <row r="94" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B94" t="s">
         <v>170</v>
@@ -4890,7 +4893,7 @@
         <v>262</v>
       </c>
       <c r="H94" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="J94" t="s">
         <v>184</v>
@@ -4898,7 +4901,7 @@
     </row>
     <row r="95" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B95" t="s">
         <v>170</v>
@@ -4913,7 +4916,7 @@
         <v>262</v>
       </c>
       <c r="H95" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="J95" t="s">
         <v>185</v>
@@ -4921,7 +4924,7 @@
     </row>
     <row r="96" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B96" t="s">
         <v>170</v>
@@ -4936,7 +4939,7 @@
         <v>262</v>
       </c>
       <c r="H96" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="J96" t="s">
         <v>186</v>
@@ -4944,7 +4947,7 @@
     </row>
     <row r="97" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B97" t="s">
         <v>170</v>
@@ -4959,7 +4962,7 @@
         <v>262</v>
       </c>
       <c r="H97" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="J97" t="s">
         <v>187</v>
@@ -4976,10 +4979,10 @@
         <v>0.98199999999999998</v>
       </c>
       <c r="F98" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H98" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="J98" t="s">
         <v>188</v>
@@ -4996,19 +4999,19 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="F99" t="s">
         <v>82</v>
       </c>
       <c r="G99" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H99" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I99" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="J99" t="s">
         <v>189</v>
@@ -5025,19 +5028,19 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="F100" t="s">
         <v>80</v>
       </c>
       <c r="G100" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="H100" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="I100" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J100" t="s">
         <v>190</v>
@@ -5054,10 +5057,10 @@
         <v>0.73</v>
       </c>
       <c r="F101" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H101" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="J101" t="s">
         <v>191</v>
@@ -5077,10 +5080,10 @@
         <v>80</v>
       </c>
       <c r="G102" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="H102" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J102" t="s">
         <v>192</v>
@@ -5100,7 +5103,7 @@
         <v>80</v>
       </c>
       <c r="H103" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="J103" t="s">
         <v>193</v>
@@ -5108,7 +5111,7 @@
     </row>
     <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B104" t="s">
         <v>170</v>
@@ -5120,10 +5123,10 @@
         <v>80</v>
       </c>
       <c r="G104" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H104" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="J104" t="s">
         <v>194</v>
@@ -5131,7 +5134,7 @@
     </row>
     <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B105" t="s">
         <v>170</v>
@@ -5143,7 +5146,7 @@
         <v>80</v>
       </c>
       <c r="H105" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="J105" t="s">
         <v>195</v>
@@ -5163,7 +5166,7 @@
         <v>81</v>
       </c>
       <c r="H106" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="J106" t="s">
         <v>196</v>
@@ -5183,10 +5186,10 @@
         <v>82</v>
       </c>
       <c r="G107" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H107" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="J107" t="s">
         <v>197</v>
@@ -5203,19 +5206,19 @@
         <v>0.125</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F108" t="s">
         <v>80</v>
       </c>
       <c r="G108" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H108" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="I108" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="J108" t="s">
         <v>198</v>
@@ -5223,7 +5226,7 @@
     </row>
     <row r="109" spans="1:10" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B109" t="s">
         <v>170</v>
@@ -5238,10 +5241,10 @@
         <v>262</v>
       </c>
       <c r="H109" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="I109" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="J109" t="s">
         <v>199</v>
@@ -5249,7 +5252,7 @@
     </row>
     <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B110" t="s">
         <v>170</v>
@@ -5264,7 +5267,7 @@
         <v>262</v>
       </c>
       <c r="H110" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="J110" t="s">
         <v>200</v>
@@ -5272,7 +5275,7 @@
     </row>
     <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B111" t="s">
         <v>170</v>
@@ -5287,7 +5290,7 @@
         <v>262</v>
       </c>
       <c r="H111" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="J111" t="s">
         <v>201</v>
@@ -5295,7 +5298,7 @@
     </row>
     <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B112" t="s">
         <v>170</v>
@@ -5310,7 +5313,7 @@
         <v>262</v>
       </c>
       <c r="H112" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="J112" t="s">
         <v>202</v>
@@ -5318,7 +5321,7 @@
     </row>
     <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B113" t="s">
         <v>170</v>
@@ -5333,7 +5336,7 @@
         <v>262</v>
       </c>
       <c r="H113" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="J113" t="s">
         <v>203</v>
@@ -5341,7 +5344,7 @@
     </row>
     <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B114" t="s">
         <v>170</v>
@@ -5356,7 +5359,7 @@
         <v>262</v>
       </c>
       <c r="H114" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="J114" t="s">
         <v>204</v>
@@ -5364,7 +5367,7 @@
     </row>
     <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B115" t="s">
         <v>170</v>
@@ -5379,7 +5382,7 @@
         <v>262</v>
       </c>
       <c r="H115" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="J115" t="s">
         <v>205</v>
@@ -5399,7 +5402,7 @@
         <v>81</v>
       </c>
       <c r="H116" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J116" t="s">
         <v>206</v>
@@ -5416,19 +5419,19 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F117" t="s">
         <v>80</v>
       </c>
       <c r="G117" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H117" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I117" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="J117" t="s">
         <v>207</v>
@@ -5445,10 +5448,10 @@
         <v>0.77300000000000002</v>
       </c>
       <c r="F118" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H118" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="J118" t="s">
         <v>208</v>
@@ -5465,10 +5468,10 @@
         <v>0.77300000000000002</v>
       </c>
       <c r="F119" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H119" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="J119" t="s">
         <v>209</v>
@@ -5488,7 +5491,7 @@
         <v>81</v>
       </c>
       <c r="H120" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="J120" t="s">
         <v>210</v>
@@ -5508,10 +5511,10 @@
         <v>80</v>
       </c>
       <c r="G121" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H121" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="J121" t="s">
         <v>211</v>
@@ -5531,7 +5534,7 @@
         <v>81</v>
       </c>
       <c r="H122" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="J122" t="s">
         <v>212</v>
@@ -5554,7 +5557,7 @@
         <v>262</v>
       </c>
       <c r="H123" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J123" t="s">
         <v>213</v>
@@ -5577,7 +5580,7 @@
         <v>262</v>
       </c>
       <c r="H124" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="J124" t="s">
         <v>214</v>
@@ -5600,7 +5603,7 @@
         <v>262</v>
       </c>
       <c r="H125" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="J125" t="s">
         <v>215</v>
@@ -5608,7 +5611,7 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B126" t="s">
         <v>168</v>
@@ -5617,12 +5620,12 @@
         <v>81</v>
       </c>
       <c r="H126" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="127" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B127" t="s">
         <v>168</v>
@@ -5631,12 +5634,12 @@
         <v>81</v>
       </c>
       <c r="H127" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="128" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A128" s="64" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B128" t="s">
         <v>168</v>
@@ -5650,7 +5653,7 @@
     </row>
     <row r="129" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A129" s="64" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B129" t="s">
         <v>168</v>
@@ -5659,15 +5662,15 @@
         <v>80</v>
       </c>
       <c r="G129" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H129" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
     </row>
     <row r="130" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B130" t="s">
         <v>168</v>
@@ -5681,24 +5684,24 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
+        <v>466</v>
+      </c>
+      <c r="B131" t="s">
+        <v>168</v>
+      </c>
+      <c r="F131" t="s">
+        <v>80</v>
+      </c>
+      <c r="G131" t="s">
+        <v>298</v>
+      </c>
+      <c r="H131" t="s">
         <v>468</v>
-      </c>
-      <c r="B131" t="s">
-        <v>168</v>
-      </c>
-      <c r="F131" t="s">
-        <v>80</v>
-      </c>
-      <c r="G131" t="s">
-        <v>300</v>
-      </c>
-      <c r="H131" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B132" t="s">
         <v>168</v>
@@ -5707,12 +5710,12 @@
         <v>81</v>
       </c>
       <c r="H132" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B133" t="s">
         <v>168</v>
@@ -5721,29 +5724,29 @@
         <v>81</v>
       </c>
       <c r="H133" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
+        <v>458</v>
+      </c>
+      <c r="B134" t="s">
+        <v>168</v>
+      </c>
+      <c r="F134" t="s">
+        <v>80</v>
+      </c>
+      <c r="G134" t="s">
+        <v>298</v>
+      </c>
+      <c r="H134" t="s">
         <v>460</v>
-      </c>
-      <c r="B134" t="s">
-        <v>168</v>
-      </c>
-      <c r="F134" t="s">
-        <v>80</v>
-      </c>
-      <c r="G134" t="s">
-        <v>300</v>
-      </c>
-      <c r="H134" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B135" t="s">
         <v>168</v>
@@ -5752,21 +5755,21 @@
         <v>81</v>
       </c>
       <c r="H135" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B136" t="s">
         <v>168</v>
       </c>
       <c r="F136" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H136" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J136" t="s">
         <v>147</v>
@@ -5783,7 +5786,7 @@
         <v>81</v>
       </c>
       <c r="H137" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="J137" t="s">
         <v>136</v>
@@ -5791,7 +5794,7 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B138" t="s">
         <v>168</v>
@@ -5800,7 +5803,7 @@
         <v>81</v>
       </c>
       <c r="H138" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="J138" t="s">
         <v>136</v>
@@ -5808,7 +5811,7 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" s="63" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B139" t="s">
         <v>170</v>
@@ -5820,12 +5823,12 @@
         <v>262</v>
       </c>
       <c r="H139" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B140" t="s">
         <v>168</v>
@@ -5834,15 +5837,15 @@
         <v>80</v>
       </c>
       <c r="G140" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H140" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B141" t="s">
         <v>168</v>
@@ -5851,12 +5854,12 @@
         <v>81</v>
       </c>
       <c r="H141" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" s="60" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B142" s="60" t="s">
         <v>168</v>
@@ -5868,15 +5871,15 @@
         <v>80</v>
       </c>
       <c r="G142" s="60" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H142" s="60" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" s="60" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B143" s="60" t="s">
         <v>168</v>
@@ -5889,12 +5892,12 @@
       </c>
       <c r="G143" s="60"/>
       <c r="H143" s="60" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" s="60" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B144" s="60" t="s">
         <v>168</v>
@@ -5906,15 +5909,15 @@
         <v>80</v>
       </c>
       <c r="G144" s="60" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H144" s="60" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="60" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B145" s="60" t="s">
         <v>168</v>
@@ -5927,12 +5930,12 @@
       </c>
       <c r="G145" s="60"/>
       <c r="H145" s="60" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" s="60" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B146" s="60" t="s">
         <v>168</v>
@@ -5944,21 +5947,21 @@
         <v>262</v>
       </c>
       <c r="H146" s="60" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B147" s="60" t="s">
         <v>168</v>
       </c>
       <c r="F147" s="60" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H147" s="60" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spelling out CNB and FNA
</commit_message>
<xml_diff>
--- a/data/Metadata.xlsx
+++ b/data/Metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yifu/Documents/github-repo/iibr-pmrt-calculator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C040D1-7D9A-424B-AB4F-48F8DEAA22E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576FC495-FB61-C04B-9C5E-97A2535EC1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3920" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{2D76DBCA-B48D-704D-8521-B15612E5208C}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{2D76DBCA-B48D-704D-8521-B15612E5208C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1749,7 +1749,7 @@
     <t>Maximum dimension/size of pre-operative tumor on any imaging modality (measured in mm)</t>
   </si>
   <si>
-    <t>1, CNB | 2, surgical biopsy | 3, FNA</t>
+    <t>1, core needle biopsy | 2, surgical biopsy | 3, fine needle aspirate</t>
   </si>
 </sst>
 </file>
@@ -2676,7 +2676,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G53" sqref="G53"/>
+      <selection pane="bottomLeft" activeCell="G56" sqref="A1:J147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3953,7 +3953,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>35</v>
       </c>
@@ -5975,8 +5975,8 @@
       <sortCondition sortBy="cellColor" ref="A1:A125" dxfId="0"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="C146:C1048576 C135:C141 C126:C132">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="C133:C134">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5985,8 +5985,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C133:C134">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="C146:C1048576 C135:C141 C126:C132">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>